<commit_message>
feat (dev #2): carga de nuevos elementos  caso de uso 2
</commit_message>
<xml_diff>
--- a/Repo/Articulo1/output/TOPSIS.xlsx
+++ b/Repo/Articulo1/output/TOPSIS.xlsx
@@ -470,7 +470,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>07/17/23</t>
+          <t>12/15/23</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -607,7 +607,7 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>3837.013636363637</v>
+        <v>3837.661363636364</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
@@ -619,7 +619,7 @@
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>281.6368009090909</v>
+        <v>281.6843440909091</v>
       </c>
       <c r="K2" t="n">
         <v>0.33</v>
@@ -663,7 +663,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>1918.506818181818</v>
+        <v>1918.830681818182</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -675,16 +675,16 @@
         <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>141.6516069987547</v>
+        <v>141.6753785896638</v>
       </c>
       <c r="K3" t="n">
         <v>0.9500000000000001</v>
       </c>
       <c r="L3" t="n">
-        <v>0.0009955431963418677</v>
+        <v>0.0009955439450257677</v>
       </c>
       <c r="M3" t="n">
-        <v>202.3432782755401</v>
+        <v>202.343378516875</v>
       </c>
       <c r="N3" t="n">
         <v>1225</v>
@@ -719,10 +719,10 @@
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>1918.506818181818</v>
+        <v>1918.830681818182</v>
       </c>
       <c r="G4" t="n">
-        <v>640.793947259624</v>
+        <v>581.4962964407727</v>
       </c>
       <c r="H4" t="n">
         <v>4.540635118306349</v>
@@ -731,16 +731,16 @@
         <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>223.5449862521488</v>
+        <v>215.9519745953764</v>
       </c>
       <c r="K4" t="n">
         <v>0.5625</v>
       </c>
       <c r="L4" t="n">
-        <v>0.0007506139335251635</v>
+        <v>0.0007682047477784525</v>
       </c>
       <c r="M4" t="n">
-        <v>183.2282421272689</v>
+        <v>184.6099362344079</v>
       </c>
       <c r="N4" t="n">
         <v>8362.5</v>
@@ -755,7 +755,7 @@
         <v>0</v>
       </c>
       <c r="R4" t="n">
-        <v>0.875</v>
+        <v>0.8541749999999999</v>
       </c>
     </row>
     <row r="5">
@@ -775,7 +775,7 @@
         <v>250</v>
       </c>
       <c r="F5" t="n">
-        <v>1918.506818181818</v>
+        <v>1918.830681818182</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
@@ -787,16 +787,16 @@
         <v>3113.856</v>
       </c>
       <c r="J5" t="n">
-        <v>941.1846101266499</v>
+        <v>941.208381717559</v>
       </c>
       <c r="K5" t="n">
         <v>39.9477784</v>
       </c>
       <c r="L5" t="n">
-        <v>0.958603951173407</v>
+        <v>0.9585423829577381</v>
       </c>
       <c r="M5" t="n">
-        <v>121.8776121123448</v>
+        <v>121.8828239398169</v>
       </c>
       <c r="N5" t="n">
         <v>1387.5</v>
@@ -831,10 +831,10 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>1918.506818181818</v>
+        <v>1918.830681818182</v>
       </c>
       <c r="G6" t="n">
-        <v>1067.989912099374</v>
+        <v>969.1604940679548</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
@@ -843,16 +843,16 @@
         <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>278.00170466371</v>
+        <v>265.3308375084833</v>
       </c>
       <c r="K6" t="n">
         <v>0.175</v>
       </c>
       <c r="L6" t="n">
-        <v>0.0006455764403994414</v>
+        <v>0.0006674037740520366</v>
       </c>
       <c r="M6" t="n">
-        <v>175.0574402764045</v>
+        <v>176.7746002046588</v>
       </c>
       <c r="N6" t="n">
         <v>15500</v>
@@ -867,7 +867,7 @@
         <v>0</v>
       </c>
       <c r="R6" t="n">
-        <v>0.9166500000000001</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="7">
@@ -887,10 +887,10 @@
         <v>250</v>
       </c>
       <c r="F7" t="n">
-        <v>1918.506818181818</v>
+        <v>1918.830681818182</v>
       </c>
       <c r="G7" t="n">
-        <v>640.793947259624</v>
+        <v>581.4962964407727</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -899,16 +899,16 @@
         <v>3113.856</v>
       </c>
       <c r="J7" t="n">
-        <v>1023.077989380044</v>
+        <v>1015.484977723272</v>
       </c>
       <c r="K7" t="n">
         <v>39.5602784</v>
       </c>
       <c r="L7" t="n">
-        <v>0.8510959963766491</v>
+        <v>0.8600362376318947</v>
       </c>
       <c r="M7" t="n">
-        <v>122.2633983069356</v>
+        <v>122.2394648325498</v>
       </c>
       <c r="N7" t="n">
         <v>8525</v>
@@ -923,7 +923,7 @@
         <v>0.125</v>
       </c>
       <c r="R7" t="n">
-        <v>0.795825</v>
+        <v>0.775</v>
       </c>
     </row>
     <row r="8">
@@ -943,7 +943,7 @@
         <v>500</v>
       </c>
       <c r="F8" t="n">
-        <v>1918.506818181818</v>
+        <v>1918.830681818182</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
@@ -955,16 +955,16 @@
         <v>5189.76</v>
       </c>
       <c r="J8" t="n">
-        <v>1474.067744454545</v>
+        <v>1474.091516045455</v>
       </c>
       <c r="K8" t="n">
         <v>65.81546400000002</v>
       </c>
       <c r="L8" t="n">
-        <v>1.131928037118369</v>
+        <v>1.131876512634409</v>
       </c>
       <c r="M8" t="n">
-        <v>107.3404408132477</v>
+        <v>107.344796278664</v>
       </c>
       <c r="N8" t="n">
         <v>1550</v>
@@ -999,10 +999,10 @@
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>959.2534090909091</v>
+        <v>959.415340909091</v>
       </c>
       <c r="G9" t="n">
-        <v>640.793947259624</v>
+        <v>581.4962964407727</v>
       </c>
       <c r="H9" t="n">
         <v>9.081270236612697</v>
@@ -1011,16 +1011,16 @@
         <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>153.5523892969807</v>
+        <v>145.9474918447538</v>
       </c>
       <c r="K9" t="n">
         <v>0.8725000000000001</v>
       </c>
       <c r="L9" t="n">
-        <v>0.0005999811623896996</v>
+        <v>0.0006226357822778281</v>
       </c>
       <c r="M9" t="n">
-        <v>171.1756420043254</v>
+        <v>172.9466370019421</v>
       </c>
       <c r="N9" t="n">
         <v>8425</v>
@@ -1035,7 +1035,7 @@
         <v>0</v>
       </c>
       <c r="R9" t="n">
-        <v>0.7916749999999999</v>
+        <v>0.7708499999999999</v>
       </c>
     </row>
     <row r="10">
@@ -1055,7 +1055,7 @@
         <v>250</v>
       </c>
       <c r="F10" t="n">
-        <v>959.2534090909091</v>
+        <v>959.415340909091</v>
       </c>
       <c r="G10" t="n">
         <v>0</v>
@@ -1067,16 +1067,16 @@
         <v>3113.856</v>
       </c>
       <c r="J10" t="n">
-        <v>871.1920131714818</v>
+        <v>871.2038989669363</v>
       </c>
       <c r="K10" t="n">
         <v>40.2577784</v>
       </c>
       <c r="L10" t="n">
-        <v>1.182560277804791</v>
+        <v>1.182513409681848</v>
       </c>
       <c r="M10" t="n">
-        <v>102.7784518394114</v>
+        <v>102.7824248773017</v>
       </c>
       <c r="N10" t="n">
         <v>1450</v>
@@ -1111,10 +1111,10 @@
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>959.2534090909091</v>
+        <v>959.415340909091</v>
       </c>
       <c r="G11" t="n">
-        <v>1067.989912099374</v>
+        <v>969.1604940679548</v>
       </c>
       <c r="H11" t="n">
         <v>4.540635118306349</v>
@@ -1123,16 +1123,16 @@
         <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>208.0091077085419</v>
+        <v>195.3263547578607</v>
       </c>
       <c r="K11" t="n">
         <v>0.485</v>
       </c>
       <c r="L11" t="n">
-        <v>0.0004769226130545392</v>
+        <v>0.0005008938046836479</v>
       </c>
       <c r="M11" t="n">
-        <v>161.6726742933793</v>
+        <v>163.5525333137287</v>
       </c>
       <c r="N11" t="n">
         <v>15562.5</v>
@@ -1147,7 +1147,7 @@
         <v>0</v>
       </c>
       <c r="R11" t="n">
-        <v>0.8333250000000001</v>
+        <v>0.7916749999999999</v>
       </c>
     </row>
     <row r="12">
@@ -1167,10 +1167,10 @@
         <v>250</v>
       </c>
       <c r="F12" t="n">
-        <v>959.2534090909091</v>
+        <v>959.415340909091</v>
       </c>
       <c r="G12" t="n">
-        <v>640.793947259624</v>
+        <v>581.4962964407727</v>
       </c>
       <c r="H12" t="n">
         <v>4.540635118306349</v>
@@ -1179,16 +1179,16 @@
         <v>3113.856</v>
       </c>
       <c r="J12" t="n">
-        <v>953.0853924248759</v>
+        <v>945.480494972649</v>
       </c>
       <c r="K12" t="n">
         <v>39.8702784</v>
       </c>
       <c r="L12" t="n">
-        <v>1.023100414119094</v>
+        <v>1.036085477403926</v>
       </c>
       <c r="M12" t="n">
-        <v>105.8177015515107</v>
+        <v>105.5773312969772</v>
       </c>
       <c r="N12" t="n">
         <v>8587.5</v>
@@ -1203,7 +1203,7 @@
         <v>0.125</v>
       </c>
       <c r="R12" t="n">
-        <v>0.7125</v>
+        <v>0.6916749999999999</v>
       </c>
     </row>
     <row r="13">
@@ -1223,7 +1223,7 @@
         <v>500</v>
       </c>
       <c r="F13" t="n">
-        <v>959.2534090909091</v>
+        <v>959.415340909091</v>
       </c>
       <c r="G13" t="n">
         <v>0</v>
@@ -1235,16 +1235,16 @@
         <v>5189.76</v>
       </c>
       <c r="J13" t="n">
-        <v>1404.075147499377</v>
+        <v>1404.087033294832</v>
       </c>
       <c r="K13" t="n">
         <v>66.12546400000001</v>
       </c>
       <c r="L13" t="n">
-        <v>1.30738877741298</v>
+        <v>1.307354400475403</v>
       </c>
       <c r="M13" t="n">
-        <v>92.41488128683751</v>
+        <v>92.41778969754377</v>
       </c>
       <c r="N13" t="n">
         <v>1612.5</v>
@@ -1279,10 +1279,10 @@
         <v>250</v>
       </c>
       <c r="F14" t="n">
-        <v>959.2534090909091</v>
+        <v>959.415340909091</v>
       </c>
       <c r="G14" t="n">
-        <v>1067.989912099374</v>
+        <v>969.1604940679548</v>
       </c>
       <c r="H14" t="n">
         <v>0</v>
@@ -1291,16 +1291,16 @@
         <v>3113.856</v>
       </c>
       <c r="J14" t="n">
-        <v>1007.542110836437</v>
+        <v>994.8593578857559</v>
       </c>
       <c r="K14" t="n">
         <v>39.4827784</v>
       </c>
       <c r="L14" t="n">
-        <v>0.9389909155463747</v>
+        <v>0.9573644223375569</v>
       </c>
       <c r="M14" t="n">
-        <v>107.4352358608177</v>
+        <v>107.0946293179235</v>
       </c>
       <c r="N14" t="n">
         <v>15725</v>
@@ -1315,7 +1315,7 @@
         <v>0.125</v>
       </c>
       <c r="R14" t="n">
-        <v>0.7541500000000001</v>
+        <v>0.7125</v>
       </c>
     </row>
     <row r="15">
@@ -1335,10 +1335,10 @@
         <v>500</v>
       </c>
       <c r="F15" t="n">
-        <v>959.2534090909091</v>
+        <v>959.415340909091</v>
       </c>
       <c r="G15" t="n">
-        <v>640.793947259624</v>
+        <v>581.4962964407727</v>
       </c>
       <c r="H15" t="n">
         <v>0</v>
@@ -1347,16 +1347,16 @@
         <v>5189.76</v>
       </c>
       <c r="J15" t="n">
-        <v>1485.968526752771</v>
+        <v>1478.363629300545</v>
       </c>
       <c r="K15" t="n">
         <v>65.73796400000002</v>
       </c>
       <c r="L15" t="n">
-        <v>1.184877940454469</v>
+        <v>1.195288230377203</v>
       </c>
       <c r="M15" t="n">
-        <v>95.49808888516999</v>
+        <v>95.24102437163253</v>
       </c>
       <c r="N15" t="n">
         <v>8750</v>
@@ -1371,7 +1371,7 @@
         <v>0.25</v>
       </c>
       <c r="R15" t="n">
-        <v>0.633325</v>
+        <v>0.6125</v>
       </c>
     </row>
     <row r="16">
@@ -1450,7 +1450,7 @@
         <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>1067.989912099374</v>
+        <v>969.1604940679548</v>
       </c>
       <c r="H17" t="n">
         <v>9.081270236612697</v>
@@ -1459,16 +1459,16 @@
         <v>0</v>
       </c>
       <c r="J17" t="n">
-        <v>138.0165107533738</v>
+        <v>125.321872007238</v>
       </c>
       <c r="K17" t="n">
         <v>0.795</v>
       </c>
       <c r="L17" t="n">
-        <v>9.280258328686273e-06</v>
+        <v>9.318674915154937e-06</v>
       </c>
       <c r="M17" t="n">
-        <v>124.5594727710923</v>
+        <v>124.5179981902684</v>
       </c>
       <c r="N17" t="n">
         <v>15625</v>
@@ -1483,7 +1483,7 @@
         <v>0</v>
       </c>
       <c r="R17" t="n">
-        <v>0.75</v>
+        <v>0.7083499999999999</v>
       </c>
     </row>
     <row r="18">
@@ -1506,7 +1506,7 @@
         <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>640.793947259624</v>
+        <v>581.4962964407727</v>
       </c>
       <c r="H18" t="n">
         <v>9.081270236612697</v>
@@ -1515,16 +1515,16 @@
         <v>3113.856</v>
       </c>
       <c r="J18" t="n">
-        <v>883.0927954697078</v>
+        <v>875.4760122220262</v>
       </c>
       <c r="K18" t="n">
         <v>40.1802784</v>
       </c>
       <c r="L18" t="n">
-        <v>1.282366543874901</v>
+        <v>1.302893513632273</v>
       </c>
       <c r="M18" t="n">
-        <v>81.02873272804024</v>
+        <v>80.32535557838129</v>
       </c>
       <c r="N18" t="n">
         <v>8650</v>
@@ -1539,7 +1539,7 @@
         <v>0.125</v>
       </c>
       <c r="R18" t="n">
-        <v>0.6291749999999999</v>
+        <v>0.6083499999999999</v>
       </c>
     </row>
     <row r="19">
@@ -1618,7 +1618,7 @@
         <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>1067.989912099374</v>
+        <v>969.1604940679548</v>
       </c>
       <c r="H20" t="n">
         <v>4.540635118306349</v>
@@ -1627,16 +1627,16 @@
         <v>3113.856</v>
       </c>
       <c r="J20" t="n">
-        <v>937.549513881269</v>
+        <v>924.8548751351332</v>
       </c>
       <c r="K20" t="n">
         <v>39.7927784</v>
       </c>
       <c r="L20" t="n">
-        <v>1.152900358308349</v>
+        <v>1.180775098226832</v>
       </c>
       <c r="M20" t="n">
-        <v>85.51782949900341</v>
+        <v>84.56395046380909</v>
       </c>
       <c r="N20" t="n">
         <v>15787.5</v>
@@ -1651,7 +1651,7 @@
         <v>0.125</v>
       </c>
       <c r="R20" t="n">
-        <v>0.670825</v>
+        <v>0.6291749999999999</v>
       </c>
     </row>
     <row r="21">
@@ -1674,7 +1674,7 @@
         <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>640.793947259624</v>
+        <v>581.4962964407727</v>
       </c>
       <c r="H21" t="n">
         <v>4.540635118306349</v>
@@ -1683,16 +1683,16 @@
         <v>5189.76</v>
       </c>
       <c r="J21" t="n">
-        <v>1415.975929797603</v>
+        <v>1408.359146549922</v>
       </c>
       <c r="K21" t="n">
         <v>66.04796400000001</v>
       </c>
       <c r="L21" t="n">
-        <v>1.378578159221931</v>
+        <v>1.392731343541186</v>
       </c>
       <c r="M21" t="n">
-        <v>77.82034940911073</v>
+        <v>77.33628399786112</v>
       </c>
       <c r="N21" t="n">
         <v>8812.5</v>
@@ -1707,7 +1707,7 @@
         <v>0.25</v>
       </c>
       <c r="R21" t="n">
-        <v>0.55</v>
+        <v>0.529175</v>
       </c>
     </row>
     <row r="22">
@@ -1730,7 +1730,7 @@
         <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>2135.979824198747</v>
+        <v>1938.32098813591</v>
       </c>
       <c r="H22" t="n">
         <v>0</v>
@@ -1739,7 +1739,7 @@
         <v>0</v>
       </c>
       <c r="J22" t="n">
-        <v>274.3666084183291</v>
+        <v>248.9773309260576</v>
       </c>
       <c r="K22" t="n">
         <v>0.02</v>
@@ -1763,7 +1763,7 @@
         <v>0</v>
       </c>
       <c r="R22" t="n">
-        <v>0.8333</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="23">
@@ -1786,7 +1786,7 @@
         <v>0</v>
       </c>
       <c r="G23" t="n">
-        <v>1067.989912099374</v>
+        <v>969.1604940679548</v>
       </c>
       <c r="H23" t="n">
         <v>0</v>
@@ -1795,16 +1795,16 @@
         <v>5189.76</v>
       </c>
       <c r="J23" t="n">
-        <v>1470.432648209164</v>
+        <v>1457.738009463029</v>
       </c>
       <c r="K23" t="n">
         <v>65.66046400000002</v>
       </c>
       <c r="L23" t="n">
-        <v>1.28546803852881</v>
+        <v>1.306095221277205</v>
       </c>
       <c r="M23" t="n">
-        <v>81.04021835940149</v>
+        <v>80.33529697618681</v>
       </c>
       <c r="N23" t="n">
         <v>15950</v>
@@ -1819,7 +1819,7 @@
         <v>0.25</v>
       </c>
       <c r="R23" t="n">
-        <v>0.5916500000000001</v>
+        <v>0.55</v>
       </c>
     </row>
     <row r="24">
@@ -1848,13 +1848,13 @@
         <v>0</v>
       </c>
       <c r="I24" t="n">
-        <v>6701.532</v>
+        <v>5491.07136</v>
       </c>
       <c r="J24" t="n">
-        <v>1721.6235708</v>
+        <v>1410.656232384</v>
       </c>
       <c r="K24" t="n">
-        <v>84.77437980000001</v>
+        <v>69.462052704</v>
       </c>
       <c r="L24" t="n">
         <v>1.55</v>
@@ -1949,16 +1949,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.06014777593876288</v>
+        <v>0.06184766540416695</v>
       </c>
       <c r="C2" t="n">
-        <v>0.001565526213971937</v>
+        <v>0.001608867390929792</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0002198582778971346</v>
+        <v>0.0002182188144982442</v>
       </c>
       <c r="E2" t="n">
-        <v>0.3345844034605377</v>
+        <v>0.3338216588921143</v>
       </c>
       <c r="F2" t="n">
         <v>0.02039745084057954</v>
@@ -1973,7 +1973,7 @@
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>0.2870341709311114</v>
+        <v>0.2957183420257789</v>
       </c>
     </row>
     <row r="3">
@@ -1981,16 +1981,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.03025183176213168</v>
+        <v>0.03110677463918376</v>
       </c>
       <c r="C3" t="n">
-        <v>0.00450681788870709</v>
+        <v>0.004631587943585765</v>
       </c>
       <c r="D3" t="n">
-        <v>0.000218878412719932</v>
+        <v>0.0002172464194644282</v>
       </c>
       <c r="E3" t="n">
-        <v>0.3336005965116349</v>
+        <v>0.3328402595956353</v>
       </c>
       <c r="F3" t="n">
         <v>0.02271534298155449</v>
@@ -2005,7 +2005,7 @@
         <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>0.2391999263454417</v>
+        <v>0.2464368803271828</v>
       </c>
     </row>
     <row r="4">
@@ -2013,16 +2013,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.04774139495238834</v>
+        <v>0.04741522114496191</v>
       </c>
       <c r="C4" t="n">
-        <v>0.002668510591997619</v>
+        <v>0.002742387598175782</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0001650286867904367</v>
+        <v>0.0001676367293521366</v>
       </c>
       <c r="E4" t="n">
-        <v>0.3020858977494591</v>
+        <v>0.3036700264203089</v>
       </c>
       <c r="F4" t="n">
         <v>0.155066984231224</v>
@@ -2037,7 +2037,7 @@
         <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>0.2511548995647225</v>
+        <v>0.2525952147998696</v>
       </c>
     </row>
     <row r="5">
@@ -2045,16 +2045,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.2010041332104988</v>
+        <v>0.2066552234414497</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1895130129549755</v>
+        <v>0.1947596303268166</v>
       </c>
       <c r="D5" t="n">
-        <v>0.2107570138903742</v>
+        <v>0.2091719824553596</v>
       </c>
       <c r="E5" t="n">
-        <v>0.2009379528126722</v>
+        <v>0.2004884521437134</v>
       </c>
       <c r="F5" t="n">
         <v>0.02572860276482192</v>
@@ -2069,7 +2069,7 @@
         <v>0.1458649914978946</v>
       </c>
       <c r="J5" t="n">
-        <v>0.216473995861971</v>
+        <v>0.2230233805972918</v>
       </c>
     </row>
     <row r="6">
@@ -2077,16 +2077,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.05937144644710108</v>
+        <v>0.05825702849263064</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0008302032952881483</v>
+        <v>0.0008531872527657989</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0001419353244371834</v>
+        <v>0.0001456400603652894</v>
       </c>
       <c r="E6" t="n">
-        <v>0.2886148084468784</v>
+        <v>0.2907814639317506</v>
       </c>
       <c r="F6" t="n">
         <v>0.2874186254808935</v>
@@ -2101,7 +2101,7 @@
         <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>0.2631098727840033</v>
+        <v>0.2587535492725565</v>
       </c>
     </row>
     <row r="7">
@@ -2109,16 +2109,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.2184936964007554</v>
+        <v>0.2229636699472279</v>
       </c>
       <c r="C7" t="n">
-        <v>0.187674705658266</v>
+        <v>0.1928704299814067</v>
       </c>
       <c r="D7" t="n">
-        <v>0.187120500088516</v>
+        <v>0.1876760882015623</v>
       </c>
       <c r="E7" t="n">
-        <v>0.201573993237332</v>
+        <v>0.201075100682399</v>
       </c>
       <c r="F7" t="n">
         <v>0.1580802440144914</v>
@@ -2133,7 +2133,7 @@
         <v>0.1458649914978946</v>
       </c>
       <c r="J7" t="n">
-        <v>0.2284289690812518</v>
+        <v>0.2291817150699786</v>
       </c>
     </row>
     <row r="8">
@@ -2141,16 +2141,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>0.3148093435439518</v>
+        <v>0.3236570323201104</v>
       </c>
       <c r="C8" t="n">
-        <v>0.3122298005355343</v>
+        <v>0.3208737995409505</v>
       </c>
       <c r="D8" t="n">
-        <v>0.2488637489443285</v>
+        <v>0.2469967507454876</v>
       </c>
       <c r="E8" t="n">
-        <v>0.1769707172400298</v>
+        <v>0.176574445487236</v>
       </c>
       <c r="F8" t="n">
         <v>0.02874186254808935</v>
@@ -2165,7 +2165,7 @@
         <v>0.2917299829957891</v>
       </c>
       <c r="J8" t="n">
-        <v>0.1937480653785003</v>
+        <v>0.1996098808674008</v>
       </c>
     </row>
     <row r="9">
@@ -2173,16 +2173,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.03279342286407274</v>
+        <v>0.03204477576247032</v>
       </c>
       <c r="C9" t="n">
-        <v>0.004139156429365196</v>
+        <v>0.004253747874503768</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0001319108251337204</v>
+        <v>0.0001358708422728545</v>
       </c>
       <c r="E9" t="n">
-        <v>0.2822149407065723</v>
+        <v>0.284484740631717</v>
       </c>
       <c r="F9" t="n">
         <v>0.1562259303017115</v>
@@ -2197,7 +2197,7 @@
         <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>0.2272377772718877</v>
+        <v>0.2279544839505716</v>
       </c>
     </row>
     <row r="10">
@@ -2205,16 +2205,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>0.1860561611221832</v>
+        <v>0.1912847780589581</v>
       </c>
       <c r="C10" t="n">
-        <v>0.1909836587923431</v>
+        <v>0.1962709906031447</v>
       </c>
       <c r="D10" t="n">
-        <v>0.2599956661877185</v>
+        <v>0.2580466743890494</v>
       </c>
       <c r="E10" t="n">
-        <v>0.1694494283891154</v>
+        <v>0.1690696736843154</v>
       </c>
       <c r="F10" t="n">
         <v>0.02688754883530939</v>
@@ -2229,7 +2229,7 @@
         <v>0.1458649914978946</v>
       </c>
       <c r="J10" t="n">
-        <v>0.1925568735691361</v>
+        <v>0.1983826497479937</v>
       </c>
     </row>
     <row r="11">
@@ -2237,16 +2237,16 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>0.04442347435878548</v>
+        <v>0.04288658311013905</v>
       </c>
       <c r="C11" t="n">
-        <v>0.002300849132655725</v>
+        <v>0.002364547529093786</v>
       </c>
       <c r="D11" t="n">
-        <v>0.0001048553843963725</v>
+        <v>0.0001093044522475807</v>
       </c>
       <c r="E11" t="n">
-        <v>0.2665475277634776</v>
+        <v>0.2690321178022898</v>
       </c>
       <c r="F11" t="n">
         <v>0.288577571551381</v>
@@ -2261,7 +2261,7 @@
         <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>0.2391927504911685</v>
+        <v>0.2341128184232585</v>
       </c>
     </row>
     <row r="12">
@@ -2269,16 +2269,16 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>0.2035457243124398</v>
+        <v>0.2075932245647363</v>
       </c>
       <c r="C12" t="n">
-        <v>0.1891453514956336</v>
+        <v>0.1943817902577346</v>
       </c>
       <c r="D12" t="n">
-        <v>0.2249370951640692</v>
+        <v>0.226093344597932</v>
       </c>
       <c r="E12" t="n">
-        <v>0.1744601978376734</v>
+        <v>0.1736670931061362</v>
       </c>
       <c r="F12" t="n">
         <v>0.1592391900849789</v>
@@ -2293,7 +2293,7 @@
         <v>0.1458649914978946</v>
       </c>
       <c r="J12" t="n">
-        <v>0.2045118467884169</v>
+        <v>0.2045409842206806</v>
       </c>
     </row>
     <row r="13">
@@ -2301,16 +2301,16 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>0.2998613714556362</v>
+        <v>0.3082865869376187</v>
       </c>
       <c r="C13" t="n">
-        <v>0.3137004463729018</v>
+        <v>0.3223851598172785</v>
       </c>
       <c r="D13" t="n">
-        <v>0.2874402451440581</v>
+        <v>0.2852893274008052</v>
       </c>
       <c r="E13" t="n">
-        <v>0.1523631513069525</v>
+        <v>0.1520205965702996</v>
       </c>
       <c r="F13" t="n">
         <v>0.02990080861857682</v>
@@ -2325,7 +2325,7 @@
         <v>0.2917299829957891</v>
       </c>
       <c r="J13" t="n">
-        <v>0.1698309430856654</v>
+        <v>0.1749691500181027</v>
       </c>
     </row>
     <row r="14">
@@ -2333,16 +2333,16 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>0.2151757758071526</v>
+        <v>0.218435031912405</v>
       </c>
       <c r="C14" t="n">
-        <v>0.1873070441989241</v>
+        <v>0.1924925899123247</v>
       </c>
       <c r="D14" t="n">
-        <v>0.2064449256530797</v>
+        <v>0.2089149292852981</v>
       </c>
       <c r="E14" t="n">
-        <v>0.1771270045389468</v>
+        <v>0.1761629388851152</v>
       </c>
       <c r="F14" t="n">
         <v>0.2915908313346484</v>
@@ -2357,7 +2357,7 @@
         <v>0.1458649914978946</v>
       </c>
       <c r="J14" t="n">
-        <v>0.2164668200076977</v>
+        <v>0.2106993186933675</v>
       </c>
     </row>
     <row r="15">
@@ -2365,16 +2365,16 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>0.3173509346458929</v>
+        <v>0.3245950334433969</v>
       </c>
       <c r="C15" t="n">
-        <v>0.3118621390761924</v>
+        <v>0.3204959594718685</v>
       </c>
       <c r="D15" t="n">
-        <v>0.2605052235066231</v>
+        <v>0.2608343806166174</v>
       </c>
       <c r="E15" t="n">
-        <v>0.1574463935215631</v>
+        <v>0.156664613926888</v>
       </c>
       <c r="F15" t="n">
         <v>0.1622524498682463</v>
@@ -2389,7 +2389,7 @@
         <v>0.2917299829957891</v>
       </c>
       <c r="J15" t="n">
-        <v>0.1817859163049462</v>
+        <v>0.1811274844907896</v>
       </c>
     </row>
     <row r="16">
@@ -2397,16 +2397,16 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>0.0003558875855004722</v>
+        <v>0.0003658838742005674</v>
       </c>
       <c r="C16" t="n">
-        <v>0.007448109563442244</v>
+        <v>0.007654308496241738</v>
       </c>
       <c r="D16" t="n">
-        <v>1.187234700644527e-05</v>
+        <v>1.178381598290519e-05</v>
       </c>
       <c r="E16" t="n">
-        <v>0.1257617931209708</v>
+        <v>0.125475096778804</v>
       </c>
       <c r="F16" t="n">
         <v>0.02503323512252944</v>
@@ -2421,7 +2421,7 @@
         <v>0</v>
       </c>
       <c r="J16" t="n">
-        <v>0.191365681759772</v>
+        <v>0.1971554186285868</v>
       </c>
     </row>
     <row r="17">
@@ -2429,16 +2429,16 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>0.02947550227046987</v>
+        <v>0.02751613772764745</v>
       </c>
       <c r="C17" t="n">
-        <v>0.003771494970023302</v>
+        <v>0.003875907805421772</v>
       </c>
       <c r="D17" t="n">
-        <v>2.040341614585504e-06</v>
+        <v>2.033510192679637e-06</v>
       </c>
       <c r="E17" t="n">
-        <v>0.2053594998150932</v>
+        <v>0.2048231236710392</v>
       </c>
       <c r="F17" t="n">
         <v>0.2897365176218685</v>
@@ -2453,7 +2453,7 @@
         <v>0</v>
       </c>
       <c r="J17" t="n">
-        <v>0.2152756281983336</v>
+        <v>0.2094720875739605</v>
       </c>
     </row>
     <row r="18">
@@ -2461,16 +2461,16 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>0.1885977522241242</v>
+        <v>0.1922227791822446</v>
       </c>
       <c r="C18" t="n">
-        <v>0.1906159973330011</v>
+        <v>0.1958931505340626</v>
       </c>
       <c r="D18" t="n">
-        <v>0.281938899969236</v>
+        <v>0.2843158779622866</v>
       </c>
       <c r="E18" t="n">
-        <v>0.1335909638463324</v>
+        <v>0.1321294148530314</v>
       </c>
       <c r="F18" t="n">
         <v>0.1603981361554664</v>
@@ -2485,7 +2485,7 @@
         <v>0.1458649914978946</v>
       </c>
       <c r="J18" t="n">
-        <v>0.180594724495582</v>
+        <v>0.1799002533713826</v>
       </c>
     </row>
     <row r="19">
@@ -2493,16 +2493,16 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>0.2849133993673206</v>
+        <v>0.2929161415551272</v>
       </c>
       <c r="C19" t="n">
-        <v>0.3151710922102694</v>
+        <v>0.3238965200936065</v>
       </c>
       <c r="D19" t="n">
-        <v>0.340185080703497</v>
+        <v>0.337648351161192</v>
       </c>
       <c r="E19" t="n">
-        <v>0.1187177416269694</v>
+        <v>0.118447103451176</v>
       </c>
       <c r="F19" t="n">
         <v>0.0310597546890643</v>
@@ -2517,7 +2517,7 @@
         <v>0.2917299829957891</v>
       </c>
       <c r="J19" t="n">
-        <v>0.1459138207928305</v>
+        <v>0.1503284191688047</v>
       </c>
     </row>
     <row r="20">
@@ -2525,16 +2525,16 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>0.200227803718837</v>
+        <v>0.2030645865299134</v>
       </c>
       <c r="C20" t="n">
-        <v>0.1887776900362917</v>
+        <v>0.1940039501886527</v>
       </c>
       <c r="D20" t="n">
-        <v>0.253474687364663</v>
+        <v>0.2576673421241071</v>
       </c>
       <c r="E20" t="n">
-        <v>0.1409920763189318</v>
+        <v>0.139101597646099</v>
       </c>
       <c r="F20" t="n">
         <v>0.2927497774051359</v>
@@ -2549,7 +2549,7 @@
         <v>0.1458649914978946</v>
       </c>
       <c r="J20" t="n">
-        <v>0.1925496977148629</v>
+        <v>0.1860585878440694</v>
       </c>
     </row>
     <row r="21">
@@ -2557,16 +2557,16 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>0.3024029625575773</v>
+        <v>0.3092245880609053</v>
       </c>
       <c r="C21" t="n">
-        <v>0.3133327849135599</v>
+        <v>0.3220073197481965</v>
       </c>
       <c r="D21" t="n">
-        <v>0.3030918200331355</v>
+        <v>0.3039201827021045</v>
       </c>
       <c r="E21" t="n">
-        <v>0.1283013461325413</v>
+        <v>0.1272126077496682</v>
       </c>
       <c r="F21" t="n">
         <v>0.1634113959387338</v>
@@ -2581,7 +2581,7 @@
         <v>0.2917299829957891</v>
       </c>
       <c r="J21" t="n">
-        <v>0.1578687940121113</v>
+        <v>0.1564867536414915</v>
       </c>
     </row>
     <row r="22">
@@ -2589,16 +2589,16 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>0.05859511695543927</v>
+        <v>0.05466639158109434</v>
       </c>
       <c r="C22" t="n">
-        <v>9.48803766043598e-05</v>
+        <v>9.750711460180557e-05</v>
       </c>
       <c r="D22" t="n">
-        <v>1.956738673284498e-06</v>
+        <v>1.942147449034374e-06</v>
       </c>
       <c r="E22" t="n">
-        <v>0.2060363304447788</v>
+        <v>0.2055666340383735</v>
       </c>
       <c r="F22" t="n">
         <v>0.5544398001212074</v>
@@ -2613,7 +2613,7 @@
         <v>0</v>
       </c>
       <c r="J22" t="n">
-        <v>0.2391855746368952</v>
+        <v>0.2217887565193342</v>
       </c>
     </row>
     <row r="23">
@@ -2621,16 +2621,16 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>0.31403301405229</v>
+        <v>0.3200663954085741</v>
       </c>
       <c r="C23" t="n">
-        <v>0.3114944776168505</v>
+        <v>0.3201181194027866</v>
       </c>
       <c r="D23" t="n">
-        <v>0.2826207892427517</v>
+        <v>0.2850145508089336</v>
       </c>
       <c r="E23" t="n">
-        <v>0.1336099000497293</v>
+        <v>0.1321457677351993</v>
       </c>
       <c r="F23" t="n">
         <v>0.2957630371884033</v>
@@ -2645,7 +2645,7 @@
         <v>0.2917299829957891</v>
       </c>
       <c r="J23" t="n">
-        <v>0.1698237672313921</v>
+        <v>0.1626450881141784</v>
       </c>
     </row>
     <row r="24">
@@ -2653,16 +2653,16 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>0.3676786146310353</v>
+        <v>0.3097289447958499</v>
       </c>
       <c r="C24" t="n">
-        <v>0.4021712540912516</v>
+        <v>0.3386522166742794</v>
       </c>
       <c r="D24" t="n">
-        <v>0.3407803307405586</v>
+        <v>0.3382391624722785</v>
       </c>
       <c r="E24" t="n">
-        <v>0.1187054156359452</v>
+        <v>0.1184348055594374</v>
       </c>
       <c r="F24" t="n">
         <v>0.03708627425559916</v>
@@ -2677,7 +2677,7 @@
         <v>0.5834599659915782</v>
       </c>
       <c r="J24" t="n">
-        <v>0.100461959825889</v>
+        <v>0.1035014197090226</v>
       </c>
     </row>
   </sheetData>
@@ -2809,46 +2809,54 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B2" t="n">
-        <v>0.651095603765667</v>
-      </c>
-      <c r="C2" t="n">
-        <v>13</v>
+        <v>0.6559971525283252</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>$A_{06}$</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B3" t="n">
-        <v>0.6456528882796559</v>
-      </c>
-      <c r="C3" t="n">
-        <v>21</v>
+        <v>0.6556862914393586</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>$A_{13}$</t>
+        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="B4" t="n">
-        <v>0.6443595015312608</v>
-      </c>
-      <c r="C4" t="n">
-        <v>6</v>
+        <v>0.644502543577697</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>$A_{21}$</t>
+        </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="B5" t="n">
-        <v>0.6189634769465667</v>
-      </c>
-      <c r="C5" t="n">
-        <v>22</v>
+        <v>0.6268906474075107</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>$A_{11}$</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -2856,21 +2864,25 @@
         <v>19</v>
       </c>
       <c r="B6" t="n">
-        <v>0.6158451352156784</v>
-      </c>
-      <c r="C6" t="n">
-        <v>19</v>
+        <v>0.623060647458326</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>$A_{19}$</t>
+        </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.6121330089224496</v>
-      </c>
-      <c r="C7" t="n">
-        <v>11</v>
+        <v>0.5949561580571848</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>$A_{05}$</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -2878,21 +2890,25 @@
         <v>17</v>
       </c>
       <c r="B8" t="n">
-        <v>0.5766067563698781</v>
-      </c>
-      <c r="C8" t="n">
-        <v>17</v>
+        <v>0.5929492944874826</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>$A_{17}$</t>
+        </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="B9" t="n">
-        <v>0.5614105739375657</v>
-      </c>
-      <c r="C9" t="n">
-        <v>5</v>
+        <v>0.5883710094648167</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>$A_{22}$</t>
+        </is>
       </c>
     </row>
     <row r="10">
@@ -2900,32 +2916,38 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>0.5569113818910938</v>
-      </c>
-      <c r="C10" t="n">
-        <v>12</v>
+        <v>0.5836831394744536</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>$A_{12}$</t>
+        </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B11" t="n">
-        <v>0.5214971392676947</v>
-      </c>
-      <c r="C11" t="n">
-        <v>10</v>
+        <v>0.5531312462809661</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>$A_{03}$</t>
+        </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>0.516261064615348</v>
-      </c>
-      <c r="C12" t="n">
-        <v>3</v>
+        <v>0.5516640671157687</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>$A_{10}$</t>
+        </is>
       </c>
     </row>
     <row r="13">
@@ -2933,32 +2955,38 @@
         <v>18</v>
       </c>
       <c r="B13" t="n">
-        <v>0.5155967969671299</v>
-      </c>
-      <c r="C13" t="n">
-        <v>18</v>
+        <v>0.5376334604881771</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>$A_{18}$</t>
+        </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B14" t="n">
-        <v>0.4802415859157514</v>
-      </c>
-      <c r="C14" t="n">
-        <v>16</v>
+        <v>0.5093042082692649</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>$A_{08}$</t>
+        </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B15" t="n">
-        <v>0.475886143715695</v>
-      </c>
-      <c r="C15" t="n">
-        <v>8</v>
+        <v>0.5056804072833425</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>$A_{16}$</t>
+        </is>
       </c>
     </row>
     <row r="16">
@@ -2966,32 +2994,38 @@
         <v>0</v>
       </c>
       <c r="B16" t="n">
-        <v>0.4085771840981908</v>
-      </c>
-      <c r="C16" t="n">
-        <v>0</v>
+        <v>0.4327488994624472</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>$A_{00}$</t>
+        </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="B17" t="n">
-        <v>0.4073584863335043</v>
-      </c>
-      <c r="C17" t="n">
-        <v>20</v>
+        <v>0.413562859756012</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>$A_{04}$</t>
+        </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>0.4012702982355726</v>
-      </c>
-      <c r="C18" t="n">
-        <v>4</v>
+        <v>0.4091353226482249</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>$A_{20}$</t>
+        </is>
       </c>
     </row>
     <row r="19">
@@ -2999,10 +3033,12 @@
         <v>2</v>
       </c>
       <c r="B19" t="n">
-        <v>0.3779607510006773</v>
-      </c>
-      <c r="C19" t="n">
-        <v>2</v>
+        <v>0.3924295899897636</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>$A_{02}$</t>
+        </is>
       </c>
     </row>
     <row r="20">
@@ -3010,43 +3046,51 @@
         <v>9</v>
       </c>
       <c r="B20" t="n">
-        <v>0.3743831274074745</v>
-      </c>
-      <c r="C20" t="n">
-        <v>9</v>
+        <v>0.3824125641752777</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>$A_{09}$</t>
+        </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="B21" t="n">
-        <v>0.3530585791620973</v>
-      </c>
-      <c r="C21" t="n">
-        <v>15</v>
+        <v>0.3694510101848137</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>$A_{01}$</t>
+        </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B22" t="n">
-        <v>0.3527805223648723</v>
-      </c>
-      <c r="C22" t="n">
-        <v>1</v>
+        <v>0.36151000377089</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>$A_{07}$</t>
+        </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B23" t="n">
-        <v>0.3513393441577106</v>
-      </c>
-      <c r="C23" t="n">
-        <v>7</v>
+        <v>0.3581786233471275</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>$A_{15}$</t>
+        </is>
       </c>
     </row>
     <row r="24">
@@ -3054,10 +3098,12 @@
         <v>14</v>
       </c>
       <c r="B24" t="n">
-        <v>0.3217336849476338</v>
-      </c>
-      <c r="C24" t="n">
-        <v>14</v>
+        <v>0.3324390473858094</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>$A_{14}$</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: remove old latex print parameters
</commit_message>
<xml_diff>
--- a/Repo/Articulo1/output/TOPSIS.xlsx
+++ b/Repo/Articulo1/output/TOPSIS.xlsx
@@ -470,7 +470,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>07/17/23</t>
+          <t>04/30/24</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -607,7 +607,7 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>3837.013636363637</v>
+        <v>3837.661363636364</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
@@ -619,7 +619,7 @@
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>281.6368009090909</v>
+        <v>281.6843440909091</v>
       </c>
       <c r="K2" t="n">
         <v>0.33</v>
@@ -663,7 +663,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>1918.506818181818</v>
+        <v>1918.830681818182</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -675,16 +675,16 @@
         <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>141.6516069987547</v>
+        <v>141.6753785896638</v>
       </c>
       <c r="K3" t="n">
         <v>0.9500000000000001</v>
       </c>
       <c r="L3" t="n">
-        <v>0.0009955431963418677</v>
+        <v>0.0009955439450257677</v>
       </c>
       <c r="M3" t="n">
-        <v>202.3432782755401</v>
+        <v>202.343378516875</v>
       </c>
       <c r="N3" t="n">
         <v>1225</v>
@@ -719,10 +719,10 @@
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>1918.506818181818</v>
+        <v>1918.830681818182</v>
       </c>
       <c r="G4" t="n">
-        <v>640.793947259624</v>
+        <v>581.4962964407727</v>
       </c>
       <c r="H4" t="n">
         <v>4.540635118306349</v>
@@ -731,16 +731,16 @@
         <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>223.5449862521488</v>
+        <v>215.9519745953764</v>
       </c>
       <c r="K4" t="n">
         <v>0.5625</v>
       </c>
       <c r="L4" t="n">
-        <v>0.0007506139335251635</v>
+        <v>0.0007682047477784525</v>
       </c>
       <c r="M4" t="n">
-        <v>183.2282421272689</v>
+        <v>184.6099362344079</v>
       </c>
       <c r="N4" t="n">
         <v>8362.5</v>
@@ -755,7 +755,7 @@
         <v>0</v>
       </c>
       <c r="R4" t="n">
-        <v>0.875</v>
+        <v>0.8541749999999999</v>
       </c>
     </row>
     <row r="5">
@@ -775,7 +775,7 @@
         <v>250</v>
       </c>
       <c r="F5" t="n">
-        <v>1918.506818181818</v>
+        <v>1918.830681818182</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
@@ -787,16 +787,16 @@
         <v>3113.856</v>
       </c>
       <c r="J5" t="n">
-        <v>941.1846101266499</v>
+        <v>941.208381717559</v>
       </c>
       <c r="K5" t="n">
         <v>39.9477784</v>
       </c>
       <c r="L5" t="n">
-        <v>0.958603951173407</v>
+        <v>0.9585423829577381</v>
       </c>
       <c r="M5" t="n">
-        <v>121.8776121123448</v>
+        <v>121.8828239398169</v>
       </c>
       <c r="N5" t="n">
         <v>1387.5</v>
@@ -831,10 +831,10 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>1918.506818181818</v>
+        <v>1918.830681818182</v>
       </c>
       <c r="G6" t="n">
-        <v>1067.989912099374</v>
+        <v>969.1604940679548</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
@@ -843,16 +843,16 @@
         <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>278.00170466371</v>
+        <v>265.3308375084833</v>
       </c>
       <c r="K6" t="n">
         <v>0.175</v>
       </c>
       <c r="L6" t="n">
-        <v>0.0006455764403994414</v>
+        <v>0.0006674037740520366</v>
       </c>
       <c r="M6" t="n">
-        <v>175.0574402764045</v>
+        <v>176.7746002046588</v>
       </c>
       <c r="N6" t="n">
         <v>15500</v>
@@ -867,7 +867,7 @@
         <v>0</v>
       </c>
       <c r="R6" t="n">
-        <v>0.9166500000000001</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="7">
@@ -887,10 +887,10 @@
         <v>250</v>
       </c>
       <c r="F7" t="n">
-        <v>1918.506818181818</v>
+        <v>1918.830681818182</v>
       </c>
       <c r="G7" t="n">
-        <v>640.793947259624</v>
+        <v>581.4962964407727</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -899,16 +899,16 @@
         <v>3113.856</v>
       </c>
       <c r="J7" t="n">
-        <v>1023.077989380044</v>
+        <v>1015.484977723272</v>
       </c>
       <c r="K7" t="n">
         <v>39.5602784</v>
       </c>
       <c r="L7" t="n">
-        <v>0.8510959963766491</v>
+        <v>0.8600362376318947</v>
       </c>
       <c r="M7" t="n">
-        <v>122.2633983069356</v>
+        <v>122.2394648325498</v>
       </c>
       <c r="N7" t="n">
         <v>8525</v>
@@ -923,7 +923,7 @@
         <v>0.125</v>
       </c>
       <c r="R7" t="n">
-        <v>0.795825</v>
+        <v>0.775</v>
       </c>
     </row>
     <row r="8">
@@ -943,7 +943,7 @@
         <v>500</v>
       </c>
       <c r="F8" t="n">
-        <v>1918.506818181818</v>
+        <v>1918.830681818182</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
@@ -955,16 +955,16 @@
         <v>5189.76</v>
       </c>
       <c r="J8" t="n">
-        <v>1474.067744454545</v>
+        <v>1474.091516045455</v>
       </c>
       <c r="K8" t="n">
         <v>65.81546400000002</v>
       </c>
       <c r="L8" t="n">
-        <v>1.131928037118369</v>
+        <v>1.131876512634409</v>
       </c>
       <c r="M8" t="n">
-        <v>107.3404408132477</v>
+        <v>107.344796278664</v>
       </c>
       <c r="N8" t="n">
         <v>1550</v>
@@ -999,10 +999,10 @@
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>959.2534090909091</v>
+        <v>959.415340909091</v>
       </c>
       <c r="G9" t="n">
-        <v>640.793947259624</v>
+        <v>581.4962964407727</v>
       </c>
       <c r="H9" t="n">
         <v>9.081270236612697</v>
@@ -1011,16 +1011,16 @@
         <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>153.5523892969807</v>
+        <v>145.9474918447538</v>
       </c>
       <c r="K9" t="n">
         <v>0.8725000000000001</v>
       </c>
       <c r="L9" t="n">
-        <v>0.0005999811623896996</v>
+        <v>0.0006226357822778281</v>
       </c>
       <c r="M9" t="n">
-        <v>171.1756420043254</v>
+        <v>172.9466370019421</v>
       </c>
       <c r="N9" t="n">
         <v>8425</v>
@@ -1035,7 +1035,7 @@
         <v>0</v>
       </c>
       <c r="R9" t="n">
-        <v>0.7916749999999999</v>
+        <v>0.7708499999999999</v>
       </c>
     </row>
     <row r="10">
@@ -1055,7 +1055,7 @@
         <v>250</v>
       </c>
       <c r="F10" t="n">
-        <v>959.2534090909091</v>
+        <v>959.415340909091</v>
       </c>
       <c r="G10" t="n">
         <v>0</v>
@@ -1067,16 +1067,16 @@
         <v>3113.856</v>
       </c>
       <c r="J10" t="n">
-        <v>871.1920131714818</v>
+        <v>871.2038989669363</v>
       </c>
       <c r="K10" t="n">
         <v>40.2577784</v>
       </c>
       <c r="L10" t="n">
-        <v>1.182560277804791</v>
+        <v>1.182513409681848</v>
       </c>
       <c r="M10" t="n">
-        <v>102.7784518394114</v>
+        <v>102.7824248773017</v>
       </c>
       <c r="N10" t="n">
         <v>1450</v>
@@ -1111,10 +1111,10 @@
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>959.2534090909091</v>
+        <v>959.415340909091</v>
       </c>
       <c r="G11" t="n">
-        <v>1067.989912099374</v>
+        <v>969.1604940679548</v>
       </c>
       <c r="H11" t="n">
         <v>4.540635118306349</v>
@@ -1123,16 +1123,16 @@
         <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>208.0091077085419</v>
+        <v>195.3263547578607</v>
       </c>
       <c r="K11" t="n">
         <v>0.485</v>
       </c>
       <c r="L11" t="n">
-        <v>0.0004769226130545392</v>
+        <v>0.0005008938046836479</v>
       </c>
       <c r="M11" t="n">
-        <v>161.6726742933793</v>
+        <v>163.5525333137287</v>
       </c>
       <c r="N11" t="n">
         <v>15562.5</v>
@@ -1147,7 +1147,7 @@
         <v>0</v>
       </c>
       <c r="R11" t="n">
-        <v>0.8333250000000001</v>
+        <v>0.7916749999999999</v>
       </c>
     </row>
     <row r="12">
@@ -1167,10 +1167,10 @@
         <v>250</v>
       </c>
       <c r="F12" t="n">
-        <v>959.2534090909091</v>
+        <v>959.415340909091</v>
       </c>
       <c r="G12" t="n">
-        <v>640.793947259624</v>
+        <v>581.4962964407727</v>
       </c>
       <c r="H12" t="n">
         <v>4.540635118306349</v>
@@ -1179,16 +1179,16 @@
         <v>3113.856</v>
       </c>
       <c r="J12" t="n">
-        <v>953.0853924248759</v>
+        <v>945.480494972649</v>
       </c>
       <c r="K12" t="n">
         <v>39.8702784</v>
       </c>
       <c r="L12" t="n">
-        <v>1.023100414119094</v>
+        <v>1.036085477403926</v>
       </c>
       <c r="M12" t="n">
-        <v>105.8177015515107</v>
+        <v>105.5773312969772</v>
       </c>
       <c r="N12" t="n">
         <v>8587.5</v>
@@ -1203,7 +1203,7 @@
         <v>0.125</v>
       </c>
       <c r="R12" t="n">
-        <v>0.7125</v>
+        <v>0.6916749999999999</v>
       </c>
     </row>
     <row r="13">
@@ -1223,7 +1223,7 @@
         <v>500</v>
       </c>
       <c r="F13" t="n">
-        <v>959.2534090909091</v>
+        <v>959.415340909091</v>
       </c>
       <c r="G13" t="n">
         <v>0</v>
@@ -1235,16 +1235,16 @@
         <v>5189.76</v>
       </c>
       <c r="J13" t="n">
-        <v>1404.075147499377</v>
+        <v>1404.087033294832</v>
       </c>
       <c r="K13" t="n">
         <v>66.12546400000001</v>
       </c>
       <c r="L13" t="n">
-        <v>1.30738877741298</v>
+        <v>1.307354400475403</v>
       </c>
       <c r="M13" t="n">
-        <v>92.41488128683751</v>
+        <v>92.41778969754377</v>
       </c>
       <c r="N13" t="n">
         <v>1612.5</v>
@@ -1279,10 +1279,10 @@
         <v>250</v>
       </c>
       <c r="F14" t="n">
-        <v>959.2534090909091</v>
+        <v>959.415340909091</v>
       </c>
       <c r="G14" t="n">
-        <v>1067.989912099374</v>
+        <v>969.1604940679548</v>
       </c>
       <c r="H14" t="n">
         <v>0</v>
@@ -1291,16 +1291,16 @@
         <v>3113.856</v>
       </c>
       <c r="J14" t="n">
-        <v>1007.542110836437</v>
+        <v>994.8593578857559</v>
       </c>
       <c r="K14" t="n">
         <v>39.4827784</v>
       </c>
       <c r="L14" t="n">
-        <v>0.9389909155463747</v>
+        <v>0.9573644223375569</v>
       </c>
       <c r="M14" t="n">
-        <v>107.4352358608177</v>
+        <v>107.0946293179235</v>
       </c>
       <c r="N14" t="n">
         <v>15725</v>
@@ -1315,7 +1315,7 @@
         <v>0.125</v>
       </c>
       <c r="R14" t="n">
-        <v>0.7541500000000001</v>
+        <v>0.7125</v>
       </c>
     </row>
     <row r="15">
@@ -1335,10 +1335,10 @@
         <v>500</v>
       </c>
       <c r="F15" t="n">
-        <v>959.2534090909091</v>
+        <v>959.415340909091</v>
       </c>
       <c r="G15" t="n">
-        <v>640.793947259624</v>
+        <v>581.4962964407727</v>
       </c>
       <c r="H15" t="n">
         <v>0</v>
@@ -1347,16 +1347,16 @@
         <v>5189.76</v>
       </c>
       <c r="J15" t="n">
-        <v>1485.968526752771</v>
+        <v>1478.363629300545</v>
       </c>
       <c r="K15" t="n">
         <v>65.73796400000002</v>
       </c>
       <c r="L15" t="n">
-        <v>1.184877940454469</v>
+        <v>1.195288230377203</v>
       </c>
       <c r="M15" t="n">
-        <v>95.49808888516999</v>
+        <v>95.24102437163253</v>
       </c>
       <c r="N15" t="n">
         <v>8750</v>
@@ -1371,7 +1371,7 @@
         <v>0.25</v>
       </c>
       <c r="R15" t="n">
-        <v>0.633325</v>
+        <v>0.6125</v>
       </c>
     </row>
     <row r="16">
@@ -1450,7 +1450,7 @@
         <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>1067.989912099374</v>
+        <v>969.1604940679548</v>
       </c>
       <c r="H17" t="n">
         <v>9.081270236612697</v>
@@ -1459,16 +1459,16 @@
         <v>0</v>
       </c>
       <c r="J17" t="n">
-        <v>138.0165107533738</v>
+        <v>125.321872007238</v>
       </c>
       <c r="K17" t="n">
         <v>0.795</v>
       </c>
       <c r="L17" t="n">
-        <v>9.280258328686273e-06</v>
+        <v>9.318674915154937e-06</v>
       </c>
       <c r="M17" t="n">
-        <v>124.5594727710923</v>
+        <v>124.5179981902684</v>
       </c>
       <c r="N17" t="n">
         <v>15625</v>
@@ -1483,7 +1483,7 @@
         <v>0</v>
       </c>
       <c r="R17" t="n">
-        <v>0.75</v>
+        <v>0.7083499999999999</v>
       </c>
     </row>
     <row r="18">
@@ -1506,7 +1506,7 @@
         <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>640.793947259624</v>
+        <v>581.4962964407727</v>
       </c>
       <c r="H18" t="n">
         <v>9.081270236612697</v>
@@ -1515,16 +1515,16 @@
         <v>3113.856</v>
       </c>
       <c r="J18" t="n">
-        <v>883.0927954697078</v>
+        <v>875.4760122220262</v>
       </c>
       <c r="K18" t="n">
         <v>40.1802784</v>
       </c>
       <c r="L18" t="n">
-        <v>1.282366543874901</v>
+        <v>1.302893513632273</v>
       </c>
       <c r="M18" t="n">
-        <v>81.02873272804024</v>
+        <v>80.32535557838129</v>
       </c>
       <c r="N18" t="n">
         <v>8650</v>
@@ -1539,7 +1539,7 @@
         <v>0.125</v>
       </c>
       <c r="R18" t="n">
-        <v>0.6291749999999999</v>
+        <v>0.6083499999999999</v>
       </c>
     </row>
     <row r="19">
@@ -1618,7 +1618,7 @@
         <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>1067.989912099374</v>
+        <v>969.1604940679548</v>
       </c>
       <c r="H20" t="n">
         <v>4.540635118306349</v>
@@ -1627,16 +1627,16 @@
         <v>3113.856</v>
       </c>
       <c r="J20" t="n">
-        <v>937.549513881269</v>
+        <v>924.8548751351332</v>
       </c>
       <c r="K20" t="n">
         <v>39.7927784</v>
       </c>
       <c r="L20" t="n">
-        <v>1.152900358308349</v>
+        <v>1.180775098226832</v>
       </c>
       <c r="M20" t="n">
-        <v>85.51782949900341</v>
+        <v>84.56395046380909</v>
       </c>
       <c r="N20" t="n">
         <v>15787.5</v>
@@ -1651,7 +1651,7 @@
         <v>0.125</v>
       </c>
       <c r="R20" t="n">
-        <v>0.670825</v>
+        <v>0.6291749999999999</v>
       </c>
     </row>
     <row r="21">
@@ -1674,7 +1674,7 @@
         <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>640.793947259624</v>
+        <v>581.4962964407727</v>
       </c>
       <c r="H21" t="n">
         <v>4.540635118306349</v>
@@ -1683,16 +1683,16 @@
         <v>5189.76</v>
       </c>
       <c r="J21" t="n">
-        <v>1415.975929797603</v>
+        <v>1408.359146549922</v>
       </c>
       <c r="K21" t="n">
         <v>66.04796400000001</v>
       </c>
       <c r="L21" t="n">
-        <v>1.378578159221931</v>
+        <v>1.392731343541186</v>
       </c>
       <c r="M21" t="n">
-        <v>77.82034940911073</v>
+        <v>77.33628399786112</v>
       </c>
       <c r="N21" t="n">
         <v>8812.5</v>
@@ -1707,7 +1707,7 @@
         <v>0.25</v>
       </c>
       <c r="R21" t="n">
-        <v>0.55</v>
+        <v>0.529175</v>
       </c>
     </row>
     <row r="22">
@@ -1730,7 +1730,7 @@
         <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>2135.979824198747</v>
+        <v>1938.32098813591</v>
       </c>
       <c r="H22" t="n">
         <v>0</v>
@@ -1739,7 +1739,7 @@
         <v>0</v>
       </c>
       <c r="J22" t="n">
-        <v>274.3666084183291</v>
+        <v>248.9773309260576</v>
       </c>
       <c r="K22" t="n">
         <v>0.02</v>
@@ -1763,7 +1763,7 @@
         <v>0</v>
       </c>
       <c r="R22" t="n">
-        <v>0.8333</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="23">
@@ -1786,7 +1786,7 @@
         <v>0</v>
       </c>
       <c r="G23" t="n">
-        <v>1067.989912099374</v>
+        <v>969.1604940679548</v>
       </c>
       <c r="H23" t="n">
         <v>0</v>
@@ -1795,16 +1795,16 @@
         <v>5189.76</v>
       </c>
       <c r="J23" t="n">
-        <v>1470.432648209164</v>
+        <v>1457.738009463029</v>
       </c>
       <c r="K23" t="n">
         <v>65.66046400000002</v>
       </c>
       <c r="L23" t="n">
-        <v>1.28546803852881</v>
+        <v>1.306095221277205</v>
       </c>
       <c r="M23" t="n">
-        <v>81.04021835940149</v>
+        <v>80.33529697618681</v>
       </c>
       <c r="N23" t="n">
         <v>15950</v>
@@ -1819,7 +1819,7 @@
         <v>0.25</v>
       </c>
       <c r="R23" t="n">
-        <v>0.5916500000000001</v>
+        <v>0.55</v>
       </c>
     </row>
     <row r="24">
@@ -1848,13 +1848,13 @@
         <v>0</v>
       </c>
       <c r="I24" t="n">
-        <v>6701.532</v>
+        <v>5491.07136</v>
       </c>
       <c r="J24" t="n">
-        <v>1721.6235708</v>
+        <v>1410.656232384</v>
       </c>
       <c r="K24" t="n">
-        <v>84.77437980000001</v>
+        <v>69.462052704</v>
       </c>
       <c r="L24" t="n">
         <v>1.55</v>
@@ -1949,16 +1949,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.06014777593876288</v>
+        <v>0.06184766540416695</v>
       </c>
       <c r="C2" t="n">
-        <v>0.001565526213971937</v>
+        <v>0.001608867390929792</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0002198582778971346</v>
+        <v>0.0002182188144982442</v>
       </c>
       <c r="E2" t="n">
-        <v>0.3345844034605377</v>
+        <v>0.3338216588921143</v>
       </c>
       <c r="F2" t="n">
         <v>0.02039745084057954</v>
@@ -1973,7 +1973,7 @@
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>0.2870341709311114</v>
+        <v>0.2957183420257789</v>
       </c>
     </row>
     <row r="3">
@@ -1981,16 +1981,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.03025183176213168</v>
+        <v>0.03110677463918376</v>
       </c>
       <c r="C3" t="n">
-        <v>0.00450681788870709</v>
+        <v>0.004631587943585765</v>
       </c>
       <c r="D3" t="n">
-        <v>0.000218878412719932</v>
+        <v>0.0002172464194644282</v>
       </c>
       <c r="E3" t="n">
-        <v>0.3336005965116349</v>
+        <v>0.3328402595956353</v>
       </c>
       <c r="F3" t="n">
         <v>0.02271534298155449</v>
@@ -2005,7 +2005,7 @@
         <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>0.2391999263454417</v>
+        <v>0.2464368803271828</v>
       </c>
     </row>
     <row r="4">
@@ -2013,16 +2013,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.04774139495238834</v>
+        <v>0.04741522114496191</v>
       </c>
       <c r="C4" t="n">
-        <v>0.002668510591997619</v>
+        <v>0.002742387598175782</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0001650286867904367</v>
+        <v>0.0001676367293521366</v>
       </c>
       <c r="E4" t="n">
-        <v>0.3020858977494591</v>
+        <v>0.3036700264203089</v>
       </c>
       <c r="F4" t="n">
         <v>0.155066984231224</v>
@@ -2037,7 +2037,7 @@
         <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>0.2511548995647225</v>
+        <v>0.2525952147998696</v>
       </c>
     </row>
     <row r="5">
@@ -2045,16 +2045,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.2010041332104988</v>
+        <v>0.2066552234414497</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1895130129549755</v>
+        <v>0.1947596303268166</v>
       </c>
       <c r="D5" t="n">
-        <v>0.2107570138903742</v>
+        <v>0.2091719824553596</v>
       </c>
       <c r="E5" t="n">
-        <v>0.2009379528126722</v>
+        <v>0.2004884521437134</v>
       </c>
       <c r="F5" t="n">
         <v>0.02572860276482192</v>
@@ -2069,7 +2069,7 @@
         <v>0.1458649914978946</v>
       </c>
       <c r="J5" t="n">
-        <v>0.216473995861971</v>
+        <v>0.2230233805972918</v>
       </c>
     </row>
     <row r="6">
@@ -2077,16 +2077,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.05937144644710108</v>
+        <v>0.05825702849263064</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0008302032952881483</v>
+        <v>0.0008531872527657989</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0001419353244371834</v>
+        <v>0.0001456400603652894</v>
       </c>
       <c r="E6" t="n">
-        <v>0.2886148084468784</v>
+        <v>0.2907814639317506</v>
       </c>
       <c r="F6" t="n">
         <v>0.2874186254808935</v>
@@ -2101,7 +2101,7 @@
         <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>0.2631098727840033</v>
+        <v>0.2587535492725565</v>
       </c>
     </row>
     <row r="7">
@@ -2109,16 +2109,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.2184936964007554</v>
+        <v>0.2229636699472279</v>
       </c>
       <c r="C7" t="n">
-        <v>0.187674705658266</v>
+        <v>0.1928704299814067</v>
       </c>
       <c r="D7" t="n">
-        <v>0.187120500088516</v>
+        <v>0.1876760882015623</v>
       </c>
       <c r="E7" t="n">
-        <v>0.201573993237332</v>
+        <v>0.201075100682399</v>
       </c>
       <c r="F7" t="n">
         <v>0.1580802440144914</v>
@@ -2133,7 +2133,7 @@
         <v>0.1458649914978946</v>
       </c>
       <c r="J7" t="n">
-        <v>0.2284289690812518</v>
+        <v>0.2291817150699786</v>
       </c>
     </row>
     <row r="8">
@@ -2141,16 +2141,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>0.3148093435439518</v>
+        <v>0.3236570323201104</v>
       </c>
       <c r="C8" t="n">
-        <v>0.3122298005355343</v>
+        <v>0.3208737995409505</v>
       </c>
       <c r="D8" t="n">
-        <v>0.2488637489443285</v>
+        <v>0.2469967507454876</v>
       </c>
       <c r="E8" t="n">
-        <v>0.1769707172400298</v>
+        <v>0.176574445487236</v>
       </c>
       <c r="F8" t="n">
         <v>0.02874186254808935</v>
@@ -2165,7 +2165,7 @@
         <v>0.2917299829957891</v>
       </c>
       <c r="J8" t="n">
-        <v>0.1937480653785003</v>
+        <v>0.1996098808674008</v>
       </c>
     </row>
     <row r="9">
@@ -2173,16 +2173,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.03279342286407274</v>
+        <v>0.03204477576247032</v>
       </c>
       <c r="C9" t="n">
-        <v>0.004139156429365196</v>
+        <v>0.004253747874503768</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0001319108251337204</v>
+        <v>0.0001358708422728545</v>
       </c>
       <c r="E9" t="n">
-        <v>0.2822149407065723</v>
+        <v>0.284484740631717</v>
       </c>
       <c r="F9" t="n">
         <v>0.1562259303017115</v>
@@ -2197,7 +2197,7 @@
         <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>0.2272377772718877</v>
+        <v>0.2279544839505716</v>
       </c>
     </row>
     <row r="10">
@@ -2205,16 +2205,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>0.1860561611221832</v>
+        <v>0.1912847780589581</v>
       </c>
       <c r="C10" t="n">
-        <v>0.1909836587923431</v>
+        <v>0.1962709906031447</v>
       </c>
       <c r="D10" t="n">
-        <v>0.2599956661877185</v>
+        <v>0.2580466743890494</v>
       </c>
       <c r="E10" t="n">
-        <v>0.1694494283891154</v>
+        <v>0.1690696736843154</v>
       </c>
       <c r="F10" t="n">
         <v>0.02688754883530939</v>
@@ -2229,7 +2229,7 @@
         <v>0.1458649914978946</v>
       </c>
       <c r="J10" t="n">
-        <v>0.1925568735691361</v>
+        <v>0.1983826497479937</v>
       </c>
     </row>
     <row r="11">
@@ -2237,16 +2237,16 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>0.04442347435878548</v>
+        <v>0.04288658311013905</v>
       </c>
       <c r="C11" t="n">
-        <v>0.002300849132655725</v>
+        <v>0.002364547529093786</v>
       </c>
       <c r="D11" t="n">
-        <v>0.0001048553843963725</v>
+        <v>0.0001093044522475807</v>
       </c>
       <c r="E11" t="n">
-        <v>0.2665475277634776</v>
+        <v>0.2690321178022898</v>
       </c>
       <c r="F11" t="n">
         <v>0.288577571551381</v>
@@ -2261,7 +2261,7 @@
         <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>0.2391927504911685</v>
+        <v>0.2341128184232585</v>
       </c>
     </row>
     <row r="12">
@@ -2269,16 +2269,16 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>0.2035457243124398</v>
+        <v>0.2075932245647363</v>
       </c>
       <c r="C12" t="n">
-        <v>0.1891453514956336</v>
+        <v>0.1943817902577346</v>
       </c>
       <c r="D12" t="n">
-        <v>0.2249370951640692</v>
+        <v>0.226093344597932</v>
       </c>
       <c r="E12" t="n">
-        <v>0.1744601978376734</v>
+        <v>0.1736670931061362</v>
       </c>
       <c r="F12" t="n">
         <v>0.1592391900849789</v>
@@ -2293,7 +2293,7 @@
         <v>0.1458649914978946</v>
       </c>
       <c r="J12" t="n">
-        <v>0.2045118467884169</v>
+        <v>0.2045409842206806</v>
       </c>
     </row>
     <row r="13">
@@ -2301,16 +2301,16 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>0.2998613714556362</v>
+        <v>0.3082865869376187</v>
       </c>
       <c r="C13" t="n">
-        <v>0.3137004463729018</v>
+        <v>0.3223851598172785</v>
       </c>
       <c r="D13" t="n">
-        <v>0.2874402451440581</v>
+        <v>0.2852893274008052</v>
       </c>
       <c r="E13" t="n">
-        <v>0.1523631513069525</v>
+        <v>0.1520205965702996</v>
       </c>
       <c r="F13" t="n">
         <v>0.02990080861857682</v>
@@ -2325,7 +2325,7 @@
         <v>0.2917299829957891</v>
       </c>
       <c r="J13" t="n">
-        <v>0.1698309430856654</v>
+        <v>0.1749691500181027</v>
       </c>
     </row>
     <row r="14">
@@ -2333,16 +2333,16 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>0.2151757758071526</v>
+        <v>0.218435031912405</v>
       </c>
       <c r="C14" t="n">
-        <v>0.1873070441989241</v>
+        <v>0.1924925899123247</v>
       </c>
       <c r="D14" t="n">
-        <v>0.2064449256530797</v>
+        <v>0.2089149292852981</v>
       </c>
       <c r="E14" t="n">
-        <v>0.1771270045389468</v>
+        <v>0.1761629388851152</v>
       </c>
       <c r="F14" t="n">
         <v>0.2915908313346484</v>
@@ -2357,7 +2357,7 @@
         <v>0.1458649914978946</v>
       </c>
       <c r="J14" t="n">
-        <v>0.2164668200076977</v>
+        <v>0.2106993186933675</v>
       </c>
     </row>
     <row r="15">
@@ -2365,16 +2365,16 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>0.3173509346458929</v>
+        <v>0.3245950334433969</v>
       </c>
       <c r="C15" t="n">
-        <v>0.3118621390761924</v>
+        <v>0.3204959594718685</v>
       </c>
       <c r="D15" t="n">
-        <v>0.2605052235066231</v>
+        <v>0.2608343806166174</v>
       </c>
       <c r="E15" t="n">
-        <v>0.1574463935215631</v>
+        <v>0.156664613926888</v>
       </c>
       <c r="F15" t="n">
         <v>0.1622524498682463</v>
@@ -2389,7 +2389,7 @@
         <v>0.2917299829957891</v>
       </c>
       <c r="J15" t="n">
-        <v>0.1817859163049462</v>
+        <v>0.1811274844907896</v>
       </c>
     </row>
     <row r="16">
@@ -2397,16 +2397,16 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>0.0003558875855004722</v>
+        <v>0.0003658838742005674</v>
       </c>
       <c r="C16" t="n">
-        <v>0.007448109563442244</v>
+        <v>0.007654308496241738</v>
       </c>
       <c r="D16" t="n">
-        <v>1.187234700644527e-05</v>
+        <v>1.178381598290519e-05</v>
       </c>
       <c r="E16" t="n">
-        <v>0.1257617931209708</v>
+        <v>0.125475096778804</v>
       </c>
       <c r="F16" t="n">
         <v>0.02503323512252944</v>
@@ -2421,7 +2421,7 @@
         <v>0</v>
       </c>
       <c r="J16" t="n">
-        <v>0.191365681759772</v>
+        <v>0.1971554186285868</v>
       </c>
     </row>
     <row r="17">
@@ -2429,16 +2429,16 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>0.02947550227046987</v>
+        <v>0.02751613772764745</v>
       </c>
       <c r="C17" t="n">
-        <v>0.003771494970023302</v>
+        <v>0.003875907805421772</v>
       </c>
       <c r="D17" t="n">
-        <v>2.040341614585504e-06</v>
+        <v>2.033510192679637e-06</v>
       </c>
       <c r="E17" t="n">
-        <v>0.2053594998150932</v>
+        <v>0.2048231236710392</v>
       </c>
       <c r="F17" t="n">
         <v>0.2897365176218685</v>
@@ -2453,7 +2453,7 @@
         <v>0</v>
       </c>
       <c r="J17" t="n">
-        <v>0.2152756281983336</v>
+        <v>0.2094720875739605</v>
       </c>
     </row>
     <row r="18">
@@ -2461,16 +2461,16 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>0.1885977522241242</v>
+        <v>0.1922227791822446</v>
       </c>
       <c r="C18" t="n">
-        <v>0.1906159973330011</v>
+        <v>0.1958931505340626</v>
       </c>
       <c r="D18" t="n">
-        <v>0.281938899969236</v>
+        <v>0.2843158779622866</v>
       </c>
       <c r="E18" t="n">
-        <v>0.1335909638463324</v>
+        <v>0.1321294148530314</v>
       </c>
       <c r="F18" t="n">
         <v>0.1603981361554664</v>
@@ -2485,7 +2485,7 @@
         <v>0.1458649914978946</v>
       </c>
       <c r="J18" t="n">
-        <v>0.180594724495582</v>
+        <v>0.1799002533713826</v>
       </c>
     </row>
     <row r="19">
@@ -2493,16 +2493,16 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>0.2849133993673206</v>
+        <v>0.2929161415551272</v>
       </c>
       <c r="C19" t="n">
-        <v>0.3151710922102694</v>
+        <v>0.3238965200936065</v>
       </c>
       <c r="D19" t="n">
-        <v>0.340185080703497</v>
+        <v>0.337648351161192</v>
       </c>
       <c r="E19" t="n">
-        <v>0.1187177416269694</v>
+        <v>0.118447103451176</v>
       </c>
       <c r="F19" t="n">
         <v>0.0310597546890643</v>
@@ -2517,7 +2517,7 @@
         <v>0.2917299829957891</v>
       </c>
       <c r="J19" t="n">
-        <v>0.1459138207928305</v>
+        <v>0.1503284191688047</v>
       </c>
     </row>
     <row r="20">
@@ -2525,16 +2525,16 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>0.200227803718837</v>
+        <v>0.2030645865299134</v>
       </c>
       <c r="C20" t="n">
-        <v>0.1887776900362917</v>
+        <v>0.1940039501886527</v>
       </c>
       <c r="D20" t="n">
-        <v>0.253474687364663</v>
+        <v>0.2576673421241071</v>
       </c>
       <c r="E20" t="n">
-        <v>0.1409920763189318</v>
+        <v>0.139101597646099</v>
       </c>
       <c r="F20" t="n">
         <v>0.2927497774051359</v>
@@ -2549,7 +2549,7 @@
         <v>0.1458649914978946</v>
       </c>
       <c r="J20" t="n">
-        <v>0.1925496977148629</v>
+        <v>0.1860585878440694</v>
       </c>
     </row>
     <row r="21">
@@ -2557,16 +2557,16 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>0.3024029625575773</v>
+        <v>0.3092245880609053</v>
       </c>
       <c r="C21" t="n">
-        <v>0.3133327849135599</v>
+        <v>0.3220073197481965</v>
       </c>
       <c r="D21" t="n">
-        <v>0.3030918200331355</v>
+        <v>0.3039201827021045</v>
       </c>
       <c r="E21" t="n">
-        <v>0.1283013461325413</v>
+        <v>0.1272126077496682</v>
       </c>
       <c r="F21" t="n">
         <v>0.1634113959387338</v>
@@ -2581,7 +2581,7 @@
         <v>0.2917299829957891</v>
       </c>
       <c r="J21" t="n">
-        <v>0.1578687940121113</v>
+        <v>0.1564867536414915</v>
       </c>
     </row>
     <row r="22">
@@ -2589,16 +2589,16 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>0.05859511695543927</v>
+        <v>0.05466639158109434</v>
       </c>
       <c r="C22" t="n">
-        <v>9.48803766043598e-05</v>
+        <v>9.750711460180557e-05</v>
       </c>
       <c r="D22" t="n">
-        <v>1.956738673284498e-06</v>
+        <v>1.942147449034374e-06</v>
       </c>
       <c r="E22" t="n">
-        <v>0.2060363304447788</v>
+        <v>0.2055666340383735</v>
       </c>
       <c r="F22" t="n">
         <v>0.5544398001212074</v>
@@ -2613,7 +2613,7 @@
         <v>0</v>
       </c>
       <c r="J22" t="n">
-        <v>0.2391855746368952</v>
+        <v>0.2217887565193342</v>
       </c>
     </row>
     <row r="23">
@@ -2621,16 +2621,16 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>0.31403301405229</v>
+        <v>0.3200663954085741</v>
       </c>
       <c r="C23" t="n">
-        <v>0.3114944776168505</v>
+        <v>0.3201181194027866</v>
       </c>
       <c r="D23" t="n">
-        <v>0.2826207892427517</v>
+        <v>0.2850145508089336</v>
       </c>
       <c r="E23" t="n">
-        <v>0.1336099000497293</v>
+        <v>0.1321457677351993</v>
       </c>
       <c r="F23" t="n">
         <v>0.2957630371884033</v>
@@ -2645,7 +2645,7 @@
         <v>0.2917299829957891</v>
       </c>
       <c r="J23" t="n">
-        <v>0.1698237672313921</v>
+        <v>0.1626450881141784</v>
       </c>
     </row>
     <row r="24">
@@ -2653,16 +2653,16 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>0.3676786146310353</v>
+        <v>0.3097289447958499</v>
       </c>
       <c r="C24" t="n">
-        <v>0.4021712540912516</v>
+        <v>0.3386522166742794</v>
       </c>
       <c r="D24" t="n">
-        <v>0.3407803307405586</v>
+        <v>0.3382391624722785</v>
       </c>
       <c r="E24" t="n">
-        <v>0.1187054156359452</v>
+        <v>0.1184348055594374</v>
       </c>
       <c r="F24" t="n">
         <v>0.03708627425559916</v>
@@ -2677,7 +2677,7 @@
         <v>0.5834599659915782</v>
       </c>
       <c r="J24" t="n">
-        <v>0.100461959825889</v>
+        <v>0.1035014197090226</v>
       </c>
     </row>
   </sheetData>
@@ -2809,46 +2809,54 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B2" t="n">
-        <v>0.651095603765667</v>
-      </c>
-      <c r="C2" t="n">
-        <v>13</v>
+        <v>0.6559971525283252</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>$A_{06}$</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B3" t="n">
-        <v>0.6456528882796559</v>
-      </c>
-      <c r="C3" t="n">
-        <v>21</v>
+        <v>0.6556862914393586</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>$A_{13}$</t>
+        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="B4" t="n">
-        <v>0.6443595015312608</v>
-      </c>
-      <c r="C4" t="n">
-        <v>6</v>
+        <v>0.644502543577697</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>$A_{21}$</t>
+        </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="B5" t="n">
-        <v>0.6189634769465667</v>
-      </c>
-      <c r="C5" t="n">
-        <v>22</v>
+        <v>0.6268906474075107</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>$A_{11}$</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -2856,21 +2864,25 @@
         <v>19</v>
       </c>
       <c r="B6" t="n">
-        <v>0.6158451352156784</v>
-      </c>
-      <c r="C6" t="n">
-        <v>19</v>
+        <v>0.623060647458326</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>$A_{19}$</t>
+        </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.6121330089224496</v>
-      </c>
-      <c r="C7" t="n">
-        <v>11</v>
+        <v>0.5949561580571848</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>$A_{05}$</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -2878,21 +2890,25 @@
         <v>17</v>
       </c>
       <c r="B8" t="n">
-        <v>0.5766067563698781</v>
-      </c>
-      <c r="C8" t="n">
-        <v>17</v>
+        <v>0.5929492944874826</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>$A_{17}$</t>
+        </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="B9" t="n">
-        <v>0.5614105739375657</v>
-      </c>
-      <c r="C9" t="n">
-        <v>5</v>
+        <v>0.5883710094648167</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>$A_{22}$</t>
+        </is>
       </c>
     </row>
     <row r="10">
@@ -2900,32 +2916,38 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>0.5569113818910938</v>
-      </c>
-      <c r="C10" t="n">
-        <v>12</v>
+        <v>0.5836831394744536</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>$A_{12}$</t>
+        </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B11" t="n">
-        <v>0.5214971392676947</v>
-      </c>
-      <c r="C11" t="n">
-        <v>10</v>
+        <v>0.5531312462809661</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>$A_{03}$</t>
+        </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>0.516261064615348</v>
-      </c>
-      <c r="C12" t="n">
-        <v>3</v>
+        <v>0.5516640671157687</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>$A_{10}$</t>
+        </is>
       </c>
     </row>
     <row r="13">
@@ -2933,32 +2955,38 @@
         <v>18</v>
       </c>
       <c r="B13" t="n">
-        <v>0.5155967969671299</v>
-      </c>
-      <c r="C13" t="n">
-        <v>18</v>
+        <v>0.5376334604881771</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>$A_{18}$</t>
+        </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B14" t="n">
-        <v>0.4802415859157514</v>
-      </c>
-      <c r="C14" t="n">
-        <v>16</v>
+        <v>0.5093042082692649</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>$A_{08}$</t>
+        </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B15" t="n">
-        <v>0.475886143715695</v>
-      </c>
-      <c r="C15" t="n">
-        <v>8</v>
+        <v>0.5056804072833425</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>$A_{16}$</t>
+        </is>
       </c>
     </row>
     <row r="16">
@@ -2966,32 +2994,38 @@
         <v>0</v>
       </c>
       <c r="B16" t="n">
-        <v>0.4085771840981908</v>
-      </c>
-      <c r="C16" t="n">
-        <v>0</v>
+        <v>0.4327488994624472</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>$A_{00}$</t>
+        </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="B17" t="n">
-        <v>0.4073584863335043</v>
-      </c>
-      <c r="C17" t="n">
-        <v>20</v>
+        <v>0.413562859756012</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>$A_{04}$</t>
+        </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>0.4012702982355726</v>
-      </c>
-      <c r="C18" t="n">
-        <v>4</v>
+        <v>0.4091353226482249</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>$A_{20}$</t>
+        </is>
       </c>
     </row>
     <row r="19">
@@ -2999,10 +3033,12 @@
         <v>2</v>
       </c>
       <c r="B19" t="n">
-        <v>0.3779607510006773</v>
-      </c>
-      <c r="C19" t="n">
-        <v>2</v>
+        <v>0.3924295899897636</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>$A_{02}$</t>
+        </is>
       </c>
     </row>
     <row r="20">
@@ -3010,43 +3046,51 @@
         <v>9</v>
       </c>
       <c r="B20" t="n">
-        <v>0.3743831274074745</v>
-      </c>
-      <c r="C20" t="n">
-        <v>9</v>
+        <v>0.3824125641752777</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>$A_{09}$</t>
+        </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="B21" t="n">
-        <v>0.3530585791620973</v>
-      </c>
-      <c r="C21" t="n">
-        <v>15</v>
+        <v>0.3694510101848137</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>$A_{01}$</t>
+        </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B22" t="n">
-        <v>0.3527805223648723</v>
-      </c>
-      <c r="C22" t="n">
-        <v>1</v>
+        <v>0.36151000377089</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>$A_{07}$</t>
+        </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B23" t="n">
-        <v>0.3513393441577106</v>
-      </c>
-      <c r="C23" t="n">
-        <v>7</v>
+        <v>0.3581786233471275</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>$A_{15}$</t>
+        </is>
       </c>
     </row>
     <row r="24">
@@ -3054,10 +3098,12 @@
         <v>14</v>
       </c>
       <c r="B24" t="n">
-        <v>0.3217336849476338</v>
-      </c>
-      <c r="C24" t="n">
-        <v>14</v>
+        <v>0.3324390473858094</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>$A_{14}$</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: matrix dimension Topsis
</commit_message>
<xml_diff>
--- a/Repo/Articulo1/output/TOPSIS.xlsx
+++ b/Repo/Articulo1/output/TOPSIS.xlsx
@@ -470,7 +470,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>04/30/24</t>
+          <t>05/23/24</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -495,7 +495,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R24"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -544,51 +544,6 @@
           <t>biomass_generation</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>C1.1</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>C1.2</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>C1.4</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>C2.1</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>C2.2</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>C2.3</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>C3.1</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>C3.2</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>C3.3</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -607,7 +562,7 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>3837.661363636364</v>
+        <v>151.6650924657534</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
@@ -617,33 +572,6 @@
       </c>
       <c r="I2" t="n">
         <v>0</v>
-      </c>
-      <c r="J2" t="n">
-        <v>281.6843440909091</v>
-      </c>
-      <c r="K2" t="n">
-        <v>0.33</v>
-      </c>
-      <c r="L2" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="M2" t="n">
-        <v>202.94</v>
-      </c>
-      <c r="N2" t="n">
-        <v>1100</v>
-      </c>
-      <c r="O2" t="n">
-        <v>6.5</v>
-      </c>
-      <c r="P2" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R2" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -663,43 +591,16 @@
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>1918.830681818182</v>
+        <v>75.83254623287671</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>9.081270236612697</v>
+        <v>7.409284098692551</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
-      </c>
-      <c r="J3" t="n">
-        <v>141.6753785896638</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0.9500000000000001</v>
-      </c>
-      <c r="L3" t="n">
-        <v>0.0009955439450257677</v>
-      </c>
-      <c r="M3" t="n">
-        <v>202.343378516875</v>
-      </c>
-      <c r="N3" t="n">
-        <v>1225</v>
-      </c>
-      <c r="O3" t="n">
-        <v>23.25</v>
-      </c>
-      <c r="P3" t="n">
-        <v>0.325</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>0</v>
-      </c>
-      <c r="R3" t="n">
-        <v>0.8333499999999999</v>
       </c>
     </row>
     <row r="4">
@@ -719,43 +620,16 @@
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>1918.830681818182</v>
+        <v>75.83254623287671</v>
       </c>
       <c r="G4" t="n">
-        <v>581.4962964407727</v>
+        <v>179.4686510126716</v>
       </c>
       <c r="H4" t="n">
-        <v>4.540635118306349</v>
+        <v>7.409284098692551</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
-      </c>
-      <c r="J4" t="n">
-        <v>215.9519745953764</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0.5625</v>
-      </c>
-      <c r="L4" t="n">
-        <v>0.0007682047477784525</v>
-      </c>
-      <c r="M4" t="n">
-        <v>184.6099362344079</v>
-      </c>
-      <c r="N4" t="n">
-        <v>8362.5</v>
-      </c>
-      <c r="O4" t="n">
-        <v>22.5</v>
-      </c>
-      <c r="P4" t="n">
-        <v>0.4475</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R4" t="n">
-        <v>0.8541749999999999</v>
       </c>
     </row>
     <row r="5">
@@ -775,43 +649,16 @@
         <v>250</v>
       </c>
       <c r="F5" t="n">
-        <v>1918.830681818182</v>
+        <v>75.83254623287671</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>4.540635118306349</v>
+        <v>7.409284098692551</v>
       </c>
       <c r="I5" t="n">
-        <v>3113.856</v>
-      </c>
-      <c r="J5" t="n">
-        <v>941.208381717559</v>
-      </c>
-      <c r="K5" t="n">
-        <v>39.9477784</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0.9585423829577381</v>
-      </c>
-      <c r="M5" t="n">
-        <v>121.8828239398169</v>
-      </c>
-      <c r="N5" t="n">
-        <v>1387.5</v>
-      </c>
-      <c r="O5" t="n">
-        <v>18.5</v>
-      </c>
-      <c r="P5" t="n">
-        <v>0.3125</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>0.125</v>
-      </c>
-      <c r="R5" t="n">
-        <v>0.7541749999999999</v>
+        <v>109.9705838440668</v>
       </c>
     </row>
     <row r="6">
@@ -831,43 +678,16 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>1918.830681818182</v>
+        <v>75.83254623287671</v>
       </c>
       <c r="G6" t="n">
-        <v>969.1604940679548</v>
+        <v>299.1144183544525</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
       </c>
       <c r="I6" t="n">
         <v>0</v>
-      </c>
-      <c r="J6" t="n">
-        <v>265.3308375084833</v>
-      </c>
-      <c r="K6" t="n">
-        <v>0.175</v>
-      </c>
-      <c r="L6" t="n">
-        <v>0.0006674037740520366</v>
-      </c>
-      <c r="M6" t="n">
-        <v>176.7746002046588</v>
-      </c>
-      <c r="N6" t="n">
-        <v>15500</v>
-      </c>
-      <c r="O6" t="n">
-        <v>21.75</v>
-      </c>
-      <c r="P6" t="n">
-        <v>0.57</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>0</v>
-      </c>
-      <c r="R6" t="n">
-        <v>0.875</v>
       </c>
     </row>
     <row r="7">
@@ -887,43 +707,16 @@
         <v>250</v>
       </c>
       <c r="F7" t="n">
-        <v>1918.830681818182</v>
+        <v>75.83254623287671</v>
       </c>
       <c r="G7" t="n">
-        <v>581.4962964407727</v>
+        <v>179.4686510126716</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>3113.856</v>
-      </c>
-      <c r="J7" t="n">
-        <v>1015.484977723272</v>
-      </c>
-      <c r="K7" t="n">
-        <v>39.5602784</v>
-      </c>
-      <c r="L7" t="n">
-        <v>0.8600362376318947</v>
-      </c>
-      <c r="M7" t="n">
-        <v>122.2394648325498</v>
-      </c>
-      <c r="N7" t="n">
-        <v>8525</v>
-      </c>
-      <c r="O7" t="n">
-        <v>17.75</v>
-      </c>
-      <c r="P7" t="n">
-        <v>0.435</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>0.125</v>
-      </c>
-      <c r="R7" t="n">
-        <v>0.775</v>
+        <v>109.9705838440668</v>
       </c>
     </row>
     <row r="8">
@@ -943,7 +736,7 @@
         <v>500</v>
       </c>
       <c r="F8" t="n">
-        <v>1918.830681818182</v>
+        <v>75.83254623287671</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
@@ -952,34 +745,7 @@
         <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>5189.76</v>
-      </c>
-      <c r="J8" t="n">
-        <v>1474.091516045455</v>
-      </c>
-      <c r="K8" t="n">
-        <v>65.81546400000002</v>
-      </c>
-      <c r="L8" t="n">
-        <v>1.131876512634409</v>
-      </c>
-      <c r="M8" t="n">
-        <v>107.344796278664</v>
-      </c>
-      <c r="N8" t="n">
-        <v>1550</v>
-      </c>
-      <c r="O8" t="n">
-        <v>13.75</v>
-      </c>
-      <c r="P8" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="Q8" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="R8" t="n">
-        <v>0.675</v>
+        <v>109.9705838440668</v>
       </c>
     </row>
     <row r="9">
@@ -999,43 +765,16 @@
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>959.415340909091</v>
+        <v>45.49952773972603</v>
       </c>
       <c r="G9" t="n">
-        <v>581.4962964407727</v>
+        <v>179.4686510126716</v>
       </c>
       <c r="H9" t="n">
-        <v>9.081270236612697</v>
+        <v>7.409284098692551</v>
       </c>
       <c r="I9" t="n">
         <v>0</v>
-      </c>
-      <c r="J9" t="n">
-        <v>145.9474918447538</v>
-      </c>
-      <c r="K9" t="n">
-        <v>0.8725000000000001</v>
-      </c>
-      <c r="L9" t="n">
-        <v>0.0006226357822778281</v>
-      </c>
-      <c r="M9" t="n">
-        <v>172.9466370019421</v>
-      </c>
-      <c r="N9" t="n">
-        <v>8425</v>
-      </c>
-      <c r="O9" t="n">
-        <v>30.875</v>
-      </c>
-      <c r="P9" t="n">
-        <v>0.485</v>
-      </c>
-      <c r="Q9" t="n">
-        <v>0</v>
-      </c>
-      <c r="R9" t="n">
-        <v>0.7708499999999999</v>
       </c>
     </row>
     <row r="10">
@@ -1055,43 +794,16 @@
         <v>250</v>
       </c>
       <c r="F10" t="n">
-        <v>959.415340909091</v>
+        <v>45.49952773972603</v>
       </c>
       <c r="G10" t="n">
         <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>9.081270236612697</v>
+        <v>7.409284098692551</v>
       </c>
       <c r="I10" t="n">
-        <v>3113.856</v>
-      </c>
-      <c r="J10" t="n">
-        <v>871.2038989669363</v>
-      </c>
-      <c r="K10" t="n">
-        <v>40.2577784</v>
-      </c>
-      <c r="L10" t="n">
-        <v>1.182513409681848</v>
-      </c>
-      <c r="M10" t="n">
-        <v>102.7824248773017</v>
-      </c>
-      <c r="N10" t="n">
-        <v>1450</v>
-      </c>
-      <c r="O10" t="n">
-        <v>26.875</v>
-      </c>
-      <c r="P10" t="n">
-        <v>0.35</v>
-      </c>
-      <c r="Q10" t="n">
-        <v>0.125</v>
-      </c>
-      <c r="R10" t="n">
-        <v>0.6708499999999999</v>
+        <v>109.9705838440668</v>
       </c>
     </row>
     <row r="11">
@@ -1111,43 +823,16 @@
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>959.415340909091</v>
+        <v>45.49952773972603</v>
       </c>
       <c r="G11" t="n">
-        <v>969.1604940679548</v>
+        <v>299.1144183544525</v>
       </c>
       <c r="H11" t="n">
-        <v>4.540635118306349</v>
+        <v>7.409284098692551</v>
       </c>
       <c r="I11" t="n">
         <v>0</v>
-      </c>
-      <c r="J11" t="n">
-        <v>195.3263547578607</v>
-      </c>
-      <c r="K11" t="n">
-        <v>0.485</v>
-      </c>
-      <c r="L11" t="n">
-        <v>0.0005008938046836479</v>
-      </c>
-      <c r="M11" t="n">
-        <v>163.5525333137287</v>
-      </c>
-      <c r="N11" t="n">
-        <v>15562.5</v>
-      </c>
-      <c r="O11" t="n">
-        <v>30.125</v>
-      </c>
-      <c r="P11" t="n">
-        <v>0.6075</v>
-      </c>
-      <c r="Q11" t="n">
-        <v>0</v>
-      </c>
-      <c r="R11" t="n">
-        <v>0.7916749999999999</v>
       </c>
     </row>
     <row r="12">
@@ -1167,43 +852,16 @@
         <v>250</v>
       </c>
       <c r="F12" t="n">
-        <v>959.415340909091</v>
+        <v>45.49952773972603</v>
       </c>
       <c r="G12" t="n">
-        <v>581.4962964407727</v>
+        <v>179.4686510126716</v>
       </c>
       <c r="H12" t="n">
-        <v>4.540635118306349</v>
+        <v>7.409284098692551</v>
       </c>
       <c r="I12" t="n">
-        <v>3113.856</v>
-      </c>
-      <c r="J12" t="n">
-        <v>945.480494972649</v>
-      </c>
-      <c r="K12" t="n">
-        <v>39.8702784</v>
-      </c>
-      <c r="L12" t="n">
-        <v>1.036085477403926</v>
-      </c>
-      <c r="M12" t="n">
-        <v>105.5773312969772</v>
-      </c>
-      <c r="N12" t="n">
-        <v>8587.5</v>
-      </c>
-      <c r="O12" t="n">
-        <v>26.125</v>
-      </c>
-      <c r="P12" t="n">
-        <v>0.4725</v>
-      </c>
-      <c r="Q12" t="n">
-        <v>0.125</v>
-      </c>
-      <c r="R12" t="n">
-        <v>0.6916749999999999</v>
+        <v>109.9705838440668</v>
       </c>
     </row>
     <row r="13">
@@ -1223,43 +881,16 @@
         <v>500</v>
       </c>
       <c r="F13" t="n">
-        <v>959.415340909091</v>
+        <v>45.49952773972603</v>
       </c>
       <c r="G13" t="n">
         <v>0</v>
       </c>
       <c r="H13" t="n">
-        <v>4.540635118306349</v>
+        <v>7.409284098692551</v>
       </c>
       <c r="I13" t="n">
-        <v>5189.76</v>
-      </c>
-      <c r="J13" t="n">
-        <v>1404.087033294832</v>
-      </c>
-      <c r="K13" t="n">
-        <v>66.12546400000001</v>
-      </c>
-      <c r="L13" t="n">
-        <v>1.307354400475403</v>
-      </c>
-      <c r="M13" t="n">
-        <v>92.41778969754377</v>
-      </c>
-      <c r="N13" t="n">
-        <v>1612.5</v>
-      </c>
-      <c r="O13" t="n">
-        <v>22.125</v>
-      </c>
-      <c r="P13" t="n">
-        <v>0.3375</v>
-      </c>
-      <c r="Q13" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="R13" t="n">
-        <v>0.591675</v>
+        <v>109.9705838440668</v>
       </c>
     </row>
     <row r="14">
@@ -1279,43 +910,16 @@
         <v>250</v>
       </c>
       <c r="F14" t="n">
-        <v>959.415340909091</v>
+        <v>45.49952773972603</v>
       </c>
       <c r="G14" t="n">
-        <v>969.1604940679548</v>
+        <v>299.1144183544525</v>
       </c>
       <c r="H14" t="n">
         <v>0</v>
       </c>
       <c r="I14" t="n">
-        <v>3113.856</v>
-      </c>
-      <c r="J14" t="n">
-        <v>994.8593578857559</v>
-      </c>
-      <c r="K14" t="n">
-        <v>39.4827784</v>
-      </c>
-      <c r="L14" t="n">
-        <v>0.9573644223375569</v>
-      </c>
-      <c r="M14" t="n">
-        <v>107.0946293179235</v>
-      </c>
-      <c r="N14" t="n">
-        <v>15725</v>
-      </c>
-      <c r="O14" t="n">
-        <v>25.375</v>
-      </c>
-      <c r="P14" t="n">
-        <v>0.595</v>
-      </c>
-      <c r="Q14" t="n">
-        <v>0.125</v>
-      </c>
-      <c r="R14" t="n">
-        <v>0.7125</v>
+        <v>109.9705838440668</v>
       </c>
     </row>
     <row r="15">
@@ -1335,43 +939,16 @@
         <v>500</v>
       </c>
       <c r="F15" t="n">
-        <v>959.415340909091</v>
+        <v>45.49952773972603</v>
       </c>
       <c r="G15" t="n">
-        <v>581.4962964407727</v>
+        <v>179.4686510126716</v>
       </c>
       <c r="H15" t="n">
         <v>0</v>
       </c>
       <c r="I15" t="n">
-        <v>5189.76</v>
-      </c>
-      <c r="J15" t="n">
-        <v>1478.363629300545</v>
-      </c>
-      <c r="K15" t="n">
-        <v>65.73796400000002</v>
-      </c>
-      <c r="L15" t="n">
-        <v>1.195288230377203</v>
-      </c>
-      <c r="M15" t="n">
-        <v>95.24102437163253</v>
-      </c>
-      <c r="N15" t="n">
-        <v>8750</v>
-      </c>
-      <c r="O15" t="n">
-        <v>21.375</v>
-      </c>
-      <c r="P15" t="n">
-        <v>0.46</v>
-      </c>
-      <c r="Q15" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="R15" t="n">
-        <v>0.6125</v>
+        <v>109.9705838440668</v>
       </c>
     </row>
     <row r="16">
@@ -1397,37 +974,10 @@
         <v>0</v>
       </c>
       <c r="H16" t="n">
-        <v>18.16254047322539</v>
+        <v>7.409284098692551</v>
       </c>
       <c r="I16" t="n">
         <v>0</v>
-      </c>
-      <c r="J16" t="n">
-        <v>1.66641308841843</v>
-      </c>
-      <c r="K16" t="n">
-        <v>1.57</v>
-      </c>
-      <c r="L16" t="n">
-        <v>5.4e-05</v>
-      </c>
-      <c r="M16" t="n">
-        <v>76.28</v>
-      </c>
-      <c r="N16" t="n">
-        <v>1350</v>
-      </c>
-      <c r="O16" t="n">
-        <v>40</v>
-      </c>
-      <c r="P16" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="Q16" t="n">
-        <v>0</v>
-      </c>
-      <c r="R16" t="n">
-        <v>0.6667</v>
       </c>
     </row>
     <row r="17">
@@ -1450,40 +1000,13 @@
         <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>969.1604940679548</v>
+        <v>299.1144183544525</v>
       </c>
       <c r="H17" t="n">
-        <v>9.081270236612697</v>
+        <v>7.409284098692551</v>
       </c>
       <c r="I17" t="n">
         <v>0</v>
-      </c>
-      <c r="J17" t="n">
-        <v>125.321872007238</v>
-      </c>
-      <c r="K17" t="n">
-        <v>0.795</v>
-      </c>
-      <c r="L17" t="n">
-        <v>9.318674915154937e-06</v>
-      </c>
-      <c r="M17" t="n">
-        <v>124.5179981902684</v>
-      </c>
-      <c r="N17" t="n">
-        <v>15625</v>
-      </c>
-      <c r="O17" t="n">
-        <v>38.5</v>
-      </c>
-      <c r="P17" t="n">
-        <v>0.645</v>
-      </c>
-      <c r="Q17" t="n">
-        <v>0</v>
-      </c>
-      <c r="R17" t="n">
-        <v>0.7083499999999999</v>
       </c>
     </row>
     <row r="18">
@@ -1506,40 +1029,13 @@
         <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>581.4962964407727</v>
+        <v>179.4686510126716</v>
       </c>
       <c r="H18" t="n">
-        <v>9.081270236612697</v>
+        <v>7.409284098692551</v>
       </c>
       <c r="I18" t="n">
-        <v>3113.856</v>
-      </c>
-      <c r="J18" t="n">
-        <v>875.4760122220262</v>
-      </c>
-      <c r="K18" t="n">
-        <v>40.1802784</v>
-      </c>
-      <c r="L18" t="n">
-        <v>1.302893513632273</v>
-      </c>
-      <c r="M18" t="n">
-        <v>80.32535557838129</v>
-      </c>
-      <c r="N18" t="n">
-        <v>8650</v>
-      </c>
-      <c r="O18" t="n">
-        <v>34.5</v>
-      </c>
-      <c r="P18" t="n">
-        <v>0.51</v>
-      </c>
-      <c r="Q18" t="n">
-        <v>0.125</v>
-      </c>
-      <c r="R18" t="n">
-        <v>0.6083499999999999</v>
+        <v>109.9705838440668</v>
       </c>
     </row>
     <row r="19">
@@ -1565,37 +1061,10 @@
         <v>0</v>
       </c>
       <c r="H19" t="n">
-        <v>9.081270236612697</v>
+        <v>7.409284098692551</v>
       </c>
       <c r="I19" t="n">
-        <v>5189.76</v>
-      </c>
-      <c r="J19" t="n">
-        <v>1334.082550544209</v>
-      </c>
-      <c r="K19" t="n">
-        <v>66.43546400000001</v>
-      </c>
-      <c r="L19" t="n">
-        <v>1.547292573912818</v>
-      </c>
-      <c r="M19" t="n">
-        <v>72.00747624991654</v>
-      </c>
-      <c r="N19" t="n">
-        <v>1675</v>
-      </c>
-      <c r="O19" t="n">
-        <v>30.5</v>
-      </c>
-      <c r="P19" t="n">
-        <v>0.375</v>
-      </c>
-      <c r="Q19" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="R19" t="n">
-        <v>0.50835</v>
+        <v>109.9705838440668</v>
       </c>
     </row>
     <row r="20">
@@ -1618,40 +1087,13 @@
         <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>969.1604940679548</v>
+        <v>299.1144183544525</v>
       </c>
       <c r="H20" t="n">
-        <v>4.540635118306349</v>
+        <v>7.409284098692551</v>
       </c>
       <c r="I20" t="n">
-        <v>3113.856</v>
-      </c>
-      <c r="J20" t="n">
-        <v>924.8548751351332</v>
-      </c>
-      <c r="K20" t="n">
-        <v>39.7927784</v>
-      </c>
-      <c r="L20" t="n">
-        <v>1.180775098226832</v>
-      </c>
-      <c r="M20" t="n">
-        <v>84.56395046380909</v>
-      </c>
-      <c r="N20" t="n">
-        <v>15787.5</v>
-      </c>
-      <c r="O20" t="n">
-        <v>33.75</v>
-      </c>
-      <c r="P20" t="n">
-        <v>0.6325</v>
-      </c>
-      <c r="Q20" t="n">
-        <v>0.125</v>
-      </c>
-      <c r="R20" t="n">
-        <v>0.6291749999999999</v>
+        <v>109.9705838440668</v>
       </c>
     </row>
     <row r="21">
@@ -1674,40 +1116,13 @@
         <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>581.4962964407727</v>
+        <v>179.4686510126716</v>
       </c>
       <c r="H21" t="n">
-        <v>4.540635118306349</v>
+        <v>7.409284098692551</v>
       </c>
       <c r="I21" t="n">
-        <v>5189.76</v>
-      </c>
-      <c r="J21" t="n">
-        <v>1408.359146549922</v>
-      </c>
-      <c r="K21" t="n">
-        <v>66.04796400000001</v>
-      </c>
-      <c r="L21" t="n">
-        <v>1.392731343541186</v>
-      </c>
-      <c r="M21" t="n">
-        <v>77.33628399786112</v>
-      </c>
-      <c r="N21" t="n">
-        <v>8812.5</v>
-      </c>
-      <c r="O21" t="n">
-        <v>29.75</v>
-      </c>
-      <c r="P21" t="n">
-        <v>0.4975</v>
-      </c>
-      <c r="Q21" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="R21" t="n">
-        <v>0.529175</v>
+        <v>109.9705838440668</v>
       </c>
     </row>
     <row r="22">
@@ -1730,40 +1145,13 @@
         <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>1938.32098813591</v>
+        <v>598.2288367089051</v>
       </c>
       <c r="H22" t="n">
         <v>0</v>
       </c>
       <c r="I22" t="n">
         <v>0</v>
-      </c>
-      <c r="J22" t="n">
-        <v>248.9773309260576</v>
-      </c>
-      <c r="K22" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="L22" t="n">
-        <v>8.899999999999999e-06</v>
-      </c>
-      <c r="M22" t="n">
-        <v>124.97</v>
-      </c>
-      <c r="N22" t="n">
-        <v>29900</v>
-      </c>
-      <c r="O22" t="n">
-        <v>37</v>
-      </c>
-      <c r="P22" t="n">
-        <v>0.89</v>
-      </c>
-      <c r="Q22" t="n">
-        <v>0</v>
-      </c>
-      <c r="R22" t="n">
-        <v>0.75</v>
       </c>
     </row>
     <row r="23">
@@ -1786,40 +1174,13 @@
         <v>0</v>
       </c>
       <c r="G23" t="n">
-        <v>969.1604940679548</v>
+        <v>299.1144183544525</v>
       </c>
       <c r="H23" t="n">
         <v>0</v>
       </c>
       <c r="I23" t="n">
-        <v>5189.76</v>
-      </c>
-      <c r="J23" t="n">
-        <v>1457.738009463029</v>
-      </c>
-      <c r="K23" t="n">
-        <v>65.66046400000002</v>
-      </c>
-      <c r="L23" t="n">
-        <v>1.306095221277205</v>
-      </c>
-      <c r="M23" t="n">
-        <v>80.33529697618681</v>
-      </c>
-      <c r="N23" t="n">
-        <v>15950</v>
-      </c>
-      <c r="O23" t="n">
-        <v>29</v>
-      </c>
-      <c r="P23" t="n">
-        <v>0.62</v>
-      </c>
-      <c r="Q23" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="R23" t="n">
-        <v>0.55</v>
+        <v>109.9705838440668</v>
       </c>
     </row>
     <row r="24">
@@ -1848,34 +1209,7 @@
         <v>0</v>
       </c>
       <c r="I24" t="n">
-        <v>5491.07136</v>
-      </c>
-      <c r="J24" t="n">
-        <v>1410.656232384</v>
-      </c>
-      <c r="K24" t="n">
-        <v>69.462052704</v>
-      </c>
-      <c r="L24" t="n">
-        <v>1.55</v>
-      </c>
-      <c r="M24" t="n">
-        <v>72</v>
-      </c>
-      <c r="N24" t="n">
-        <v>2000</v>
-      </c>
-      <c r="O24" t="n">
-        <v>21</v>
-      </c>
-      <c r="P24" t="n">
-        <v>0.35</v>
-      </c>
-      <c r="Q24" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="R24" t="n">
-        <v>0.35</v>
+        <v>109.9705838440668</v>
       </c>
     </row>
   </sheetData>
@@ -1900,47 +1234,47 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>C1.1</t>
+          <t>Reducción de emisiones de CO2</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>C1.2</t>
+          <t>Ocupación del terreno</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>C1.4</t>
+          <t>Consumo de agua</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>C2.1</t>
+          <t>LCOE</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>C2.2</t>
+          <t>CAPEX</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>C2.3</t>
+          <t>OPEX</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>C3.1</t>
+          <t>Eficiencia de la generación</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>C3.2</t>
+          <t>Capacidad de responder a la demanda</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>C3.3</t>
+          <t>Autonomía del recurso primario</t>
         </is>
       </c>
     </row>
@@ -1949,22 +1283,22 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.06184766540416695</v>
+        <v>0.05105381942179634</v>
       </c>
       <c r="C2" t="n">
-        <v>0.001608867390929792</v>
+        <v>0.04648895864869391</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0002182188144982442</v>
+        <v>0.0003132571709710378</v>
       </c>
       <c r="E2" t="n">
-        <v>0.3338216588921143</v>
+        <v>0.337317112252536</v>
       </c>
       <c r="F2" t="n">
-        <v>0.02039745084057954</v>
+        <v>0.01325594133208014</v>
       </c>
       <c r="G2" t="n">
-        <v>0.04964547180033088</v>
+        <v>0.04907417715737528</v>
       </c>
       <c r="H2" t="n">
         <v>0.1054275896195656</v>
@@ -1973,7 +1307,7 @@
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>0.2957183420257789</v>
+        <v>0.2956878758043452</v>
       </c>
     </row>
     <row r="3">
@@ -1981,22 +1315,22 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.03110677463918376</v>
+        <v>0.02864461303828462</v>
       </c>
       <c r="C3" t="n">
-        <v>0.004631587943585765</v>
+        <v>0.1338318506553309</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0002172464194644282</v>
+        <v>0.0002868799774037635</v>
       </c>
       <c r="E3" t="n">
-        <v>0.3328402595956353</v>
+        <v>0.3185780114171409</v>
       </c>
       <c r="F3" t="n">
-        <v>0.02271534298155449</v>
+        <v>0.01352407287266085</v>
       </c>
       <c r="G3" t="n">
-        <v>0.1775780337473374</v>
+        <v>0.07158646518654961</v>
       </c>
       <c r="H3" t="n">
         <v>0.1370558665054353</v>
@@ -2005,7 +1339,7 @@
         <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>0.2464368803271828</v>
+        <v>0.2464558444829218</v>
       </c>
     </row>
     <row r="4">
@@ -2013,22 +1347,22 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.04741522114496191</v>
+        <v>0.1343679182096427</v>
       </c>
       <c r="C4" t="n">
-        <v>0.002742387598175782</v>
+        <v>0.0792425431511828</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0001676367293521366</v>
+        <v>9.280462970036676e-05</v>
       </c>
       <c r="E4" t="n">
-        <v>0.3036700264203089</v>
+        <v>0.2428453831252206</v>
       </c>
       <c r="F4" t="n">
-        <v>0.155066984231224</v>
+        <v>0.2504348589023849</v>
       </c>
       <c r="G4" t="n">
-        <v>0.1718497100780684</v>
+        <v>0.2135149499256719</v>
       </c>
       <c r="H4" t="n">
         <v>0.1887153854190225</v>
@@ -2037,7 +1371,7 @@
         <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>0.2525952147998696</v>
+        <v>0.2525913679058619</v>
       </c>
     </row>
     <row r="5">
@@ -2045,22 +1379,22 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.2066552234414497</v>
+        <v>0.1582098803580134</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1947596303268166</v>
+        <v>0.2745144833078922</v>
       </c>
       <c r="D5" t="n">
-        <v>0.2091719824553596</v>
+        <v>0.2764829718992348</v>
       </c>
       <c r="E5" t="n">
-        <v>0.2004884521437134</v>
+        <v>0.2053688436063582</v>
       </c>
       <c r="F5" t="n">
-        <v>0.02572860276482192</v>
+        <v>0.01954455990001895</v>
       </c>
       <c r="G5" t="n">
-        <v>0.141298650508634</v>
+        <v>0.1210818497814034</v>
       </c>
       <c r="H5" t="n">
         <v>0.131784487024457</v>
@@ -2069,7 +1403,7 @@
         <v>0.1458649914978946</v>
       </c>
       <c r="J5" t="n">
-        <v>0.2230233805972918</v>
+        <v>0.2230225803254274</v>
       </c>
     </row>
     <row r="6">
@@ -2077,22 +1411,22 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.05825702849263064</v>
+        <v>0.201732341894174</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0008531872527657989</v>
+        <v>0.02465323564703465</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0001456400603652894</v>
+        <v>6.55800754856158e-05</v>
       </c>
       <c r="E6" t="n">
-        <v>0.2907814639317506</v>
+        <v>0.2339296001838458</v>
       </c>
       <c r="F6" t="n">
-        <v>0.2874186254808935</v>
+        <v>0.2901267625073597</v>
       </c>
       <c r="G6" t="n">
-        <v>0.1661213864087995</v>
+        <v>0.2327731670169077</v>
       </c>
       <c r="H6" t="n">
         <v>0.2403749043326096</v>
@@ -2101,7 +1435,7 @@
         <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>0.2587535492725565</v>
+        <v>0.2587268913288021</v>
       </c>
     </row>
     <row r="7">
@@ -2109,22 +1443,22 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.2229636699472279</v>
+        <v>0.2608151153108446</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1928704299814067</v>
+        <v>0.219925175803744</v>
       </c>
       <c r="D7" t="n">
-        <v>0.1876760882015623</v>
+        <v>0.1462481826110516</v>
       </c>
       <c r="E7" t="n">
-        <v>0.201075100682399</v>
+        <v>0.2081180428951416</v>
       </c>
       <c r="F7" t="n">
-        <v>0.1580802440144914</v>
+        <v>0.187043742366802</v>
       </c>
       <c r="G7" t="n">
-        <v>0.1355703268393651</v>
+        <v>0.1951717774915859</v>
       </c>
       <c r="H7" t="n">
         <v>0.1834440059380442</v>
@@ -2133,7 +1467,7 @@
         <v>0.1458649914978946</v>
       </c>
       <c r="J7" t="n">
-        <v>0.2291817150699786</v>
+        <v>0.2291581037483676</v>
       </c>
     </row>
     <row r="8">
@@ -2141,22 +1475,22 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>0.3236570323201104</v>
+        <v>0.1550922228920195</v>
       </c>
       <c r="C8" t="n">
-        <v>0.3208737995409505</v>
+        <v>0.2192207976424002</v>
       </c>
       <c r="D8" t="n">
-        <v>0.2469967507454876</v>
+        <v>0.2875077447743895</v>
       </c>
       <c r="E8" t="n">
-        <v>0.176574445487236</v>
+        <v>0.2085019999904916</v>
       </c>
       <c r="F8" t="n">
-        <v>0.02874186254808935</v>
+        <v>0.01967519117641872</v>
       </c>
       <c r="G8" t="n">
-        <v>0.1050192672699307</v>
+        <v>0.1138679457392692</v>
       </c>
       <c r="H8" t="n">
         <v>0.1265131075434787</v>
@@ -2165,7 +1499,7 @@
         <v>0.2917299829957891</v>
       </c>
       <c r="J8" t="n">
-        <v>0.1996098808674008</v>
+        <v>0.199589316167933</v>
       </c>
     </row>
     <row r="9">
@@ -2173,22 +1507,22 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.03204477576247032</v>
+        <v>0.1241568791569281</v>
       </c>
       <c r="C9" t="n">
-        <v>0.004253747874503768</v>
+        <v>0.1229139891545013</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0001358708422728545</v>
+        <v>6.402819946062528e-05</v>
       </c>
       <c r="E9" t="n">
-        <v>0.284484740631717</v>
+        <v>0.2305138779719656</v>
       </c>
       <c r="F9" t="n">
-        <v>0.1562259303017115</v>
+        <v>0.2813947124262458</v>
       </c>
       <c r="G9" t="n">
-        <v>0.2358159910515717</v>
+        <v>0.2349807500016487</v>
       </c>
       <c r="H9" t="n">
         <v>0.2045295238619573</v>
@@ -2197,7 +1531,7 @@
         <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>0.2279544839505716</v>
+        <v>0.2279753522451502</v>
       </c>
     </row>
     <row r="10">
@@ -2205,22 +1539,22 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>0.1912847780589581</v>
+        <v>0.1479988413052988</v>
       </c>
       <c r="C10" t="n">
-        <v>0.1962709906031447</v>
+        <v>0.3181859293112107</v>
       </c>
       <c r="D10" t="n">
-        <v>0.2580466743890494</v>
+        <v>0.3279144740007727</v>
       </c>
       <c r="E10" t="n">
-        <v>0.1690696736843154</v>
+        <v>0.1807955895039561</v>
       </c>
       <c r="F10" t="n">
-        <v>0.02688754883530939</v>
+        <v>0.02071566206242945</v>
       </c>
       <c r="G10" t="n">
-        <v>0.2052649314821373</v>
+        <v>0.1344919349301618</v>
       </c>
       <c r="H10" t="n">
         <v>0.1475986254673919</v>
@@ -2229,7 +1563,7 @@
         <v>0.1458649914978946</v>
       </c>
       <c r="J10" t="n">
-        <v>0.1983826497479937</v>
+        <v>0.1984065646647157</v>
       </c>
     </row>
     <row r="11">
@@ -2237,22 +1571,22 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>0.04288658311013905</v>
+        <v>0.1946389603074533</v>
       </c>
       <c r="C11" t="n">
-        <v>0.002364547529093786</v>
+        <v>0.06832468165035317</v>
       </c>
       <c r="D11" t="n">
-        <v>0.0001093044522475807</v>
+        <v>4.321382673545467e-05</v>
       </c>
       <c r="E11" t="n">
-        <v>0.2690321178022898</v>
+        <v>0.2227665878359201</v>
       </c>
       <c r="F11" t="n">
-        <v>0.288577571551381</v>
+        <v>0.3082199173400735</v>
       </c>
       <c r="G11" t="n">
-        <v>0.2300876673823027</v>
+        <v>0.2500593571737579</v>
       </c>
       <c r="H11" t="n">
         <v>0.2561890427755445</v>
@@ -2261,7 +1595,7 @@
         <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>0.2341128184232585</v>
+        <v>0.2341108756680903</v>
       </c>
     </row>
     <row r="12">
@@ -2269,22 +1603,22 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>0.2075932245647363</v>
+        <v>0.2537221923380495</v>
       </c>
       <c r="C12" t="n">
-        <v>0.1943817902577346</v>
+        <v>0.2635966218070625</v>
       </c>
       <c r="D12" t="n">
-        <v>0.226093344597932</v>
+        <v>0.1560136616589028</v>
       </c>
       <c r="E12" t="n">
-        <v>0.1736670931061362</v>
+        <v>0.1949105836758716</v>
       </c>
       <c r="F12" t="n">
-        <v>0.1592391900849789</v>
+        <v>0.1987463283918775</v>
       </c>
       <c r="G12" t="n">
-        <v>0.1995366078128683</v>
+        <v>0.2104285616761434</v>
       </c>
       <c r="H12" t="n">
         <v>0.199258144380979</v>
@@ -2293,7 +1627,7 @@
         <v>0.1458649914978946</v>
       </c>
       <c r="J12" t="n">
-        <v>0.2045409842206806</v>
+        <v>0.2045420880876558</v>
       </c>
     </row>
     <row r="13">
@@ -2301,22 +1635,22 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>0.3082865869376187</v>
+        <v>0.1479988413052988</v>
       </c>
       <c r="C13" t="n">
-        <v>0.3223851598172785</v>
+        <v>0.2628922436457187</v>
       </c>
       <c r="D13" t="n">
-        <v>0.2852893274008052</v>
+        <v>0.3279144740007727</v>
       </c>
       <c r="E13" t="n">
-        <v>0.1520205965702996</v>
+        <v>0.1807955895039561</v>
       </c>
       <c r="F13" t="n">
-        <v>0.02990080861857682</v>
+        <v>0.02071566206242945</v>
       </c>
       <c r="G13" t="n">
-        <v>0.168985548243434</v>
+        <v>0.1344919349301618</v>
       </c>
       <c r="H13" t="n">
         <v>0.1423272459864136</v>
@@ -2325,7 +1659,7 @@
         <v>0.2917299829957891</v>
       </c>
       <c r="J13" t="n">
-        <v>0.1749691500181027</v>
+        <v>0.1749733005072213</v>
       </c>
     </row>
     <row r="14">
@@ -2333,22 +1667,22 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>0.218435031912405</v>
+        <v>0.3210866160225808</v>
       </c>
       <c r="C14" t="n">
-        <v>0.1924925899123247</v>
+        <v>0.2090073143029144</v>
       </c>
       <c r="D14" t="n">
-        <v>0.2089149292852981</v>
+        <v>0.1174943068876201</v>
       </c>
       <c r="E14" t="n">
-        <v>0.1761629388851152</v>
+        <v>0.1993917452735499</v>
       </c>
       <c r="F14" t="n">
-        <v>0.2915908313346484</v>
+        <v>0.2442467444714547</v>
       </c>
       <c r="G14" t="n">
-        <v>0.1938082841435994</v>
+        <v>0.2270745225679251</v>
       </c>
       <c r="H14" t="n">
         <v>0.2509176632945662</v>
@@ -2357,7 +1691,7 @@
         <v>0.1458649914978946</v>
       </c>
       <c r="J14" t="n">
-        <v>0.2106993186933675</v>
+        <v>0.210677611510596</v>
       </c>
     </row>
     <row r="15">
@@ -2365,22 +1699,22 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>0.3245950334433969</v>
+        <v>0.2506045348720556</v>
       </c>
       <c r="C15" t="n">
-        <v>0.3204959594718685</v>
+        <v>0.2083029361415706</v>
       </c>
       <c r="D15" t="n">
-        <v>0.2608343806166174</v>
+        <v>0.1594645026543197</v>
       </c>
       <c r="E15" t="n">
-        <v>0.156664613926888</v>
+        <v>0.1964164933225691</v>
       </c>
       <c r="F15" t="n">
-        <v>0.1622524498682463</v>
+        <v>0.2027833650702837</v>
       </c>
       <c r="G15" t="n">
-        <v>0.163257224574165</v>
+        <v>0.2084029306405552</v>
       </c>
       <c r="H15" t="n">
         <v>0.1939867649000008</v>
@@ -2389,7 +1723,7 @@
         <v>0.2917299829957891</v>
       </c>
       <c r="J15" t="n">
-        <v>0.1811274844907896</v>
+        <v>0.1811088239301615</v>
       </c>
     </row>
     <row r="16">
@@ -2397,22 +1731,22 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>0.0003658838742005674</v>
+        <v>0.003117666638272399</v>
       </c>
       <c r="C16" t="n">
-        <v>0.007654308496241738</v>
+        <v>0.221174742661968</v>
       </c>
       <c r="D16" t="n">
-        <v>1.178381598290519e-05</v>
+        <v>1.691588723243604e-05</v>
       </c>
       <c r="E16" t="n">
-        <v>0.125475096778804</v>
+        <v>0.1267889490619072</v>
       </c>
       <c r="F16" t="n">
-        <v>0.02503323512252944</v>
+        <v>0.01626865527118926</v>
       </c>
       <c r="G16" t="n">
-        <v>0.3055105956943439</v>
+        <v>0.3019949363530786</v>
       </c>
       <c r="H16" t="n">
         <v>0.168684143391305</v>
@@ -2421,7 +1755,7 @@
         <v>0</v>
       </c>
       <c r="J16" t="n">
-        <v>0.1971554186285868</v>
+        <v>0.1972238131614983</v>
       </c>
     </row>
     <row r="17">
@@ -2429,22 +1763,22 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>0.02751613772764745</v>
+        <v>0.1793226310353442</v>
       </c>
       <c r="C17" t="n">
-        <v>0.003875907805421772</v>
+        <v>0.1119961276536717</v>
       </c>
       <c r="D17" t="n">
-        <v>2.033510192679637e-06</v>
+        <v>3.129489259148024e-06</v>
       </c>
       <c r="E17" t="n">
-        <v>0.2048231236710392</v>
+        <v>0.2057627736132758</v>
       </c>
       <c r="F17" t="n">
-        <v>0.2897365176218685</v>
+        <v>0.3520042915599342</v>
       </c>
       <c r="G17" t="n">
-        <v>0.294053948355806</v>
+        <v>0.2798926819487377</v>
       </c>
       <c r="H17" t="n">
         <v>0.2720031812184793</v>
@@ -2453,7 +1787,7 @@
         <v>0</v>
       </c>
       <c r="J17" t="n">
-        <v>0.2094720875739605</v>
+        <v>0.2094948600073786</v>
       </c>
     </row>
     <row r="18">
@@ -2461,22 +1795,22 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>0.1922227791822446</v>
+        <v>0.2384058630659404</v>
       </c>
       <c r="C18" t="n">
-        <v>0.1958931505340626</v>
+        <v>0.307268067810381</v>
       </c>
       <c r="D18" t="n">
-        <v>0.2843158779622866</v>
+        <v>0.1798785327149893</v>
       </c>
       <c r="E18" t="n">
-        <v>0.1321294148530314</v>
+        <v>0.173081542406469</v>
       </c>
       <c r="F18" t="n">
-        <v>0.1603981361554664</v>
+        <v>0.2271779123780381</v>
       </c>
       <c r="G18" t="n">
-        <v>0.2635028887863716</v>
+        <v>0.2351596820014379</v>
       </c>
       <c r="H18" t="n">
         <v>0.2150722828239139</v>
@@ -2485,7 +1819,7 @@
         <v>0.1458649914978946</v>
       </c>
       <c r="J18" t="n">
-        <v>0.1799002533713826</v>
+        <v>0.1799260724269441</v>
       </c>
     </row>
     <row r="19">
@@ -2493,22 +1827,22 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>0.2929161415551272</v>
+        <v>0.1326825120331897</v>
       </c>
       <c r="C19" t="n">
-        <v>0.3238965200936065</v>
+        <v>0.3065636896490372</v>
       </c>
       <c r="D19" t="n">
-        <v>0.337648351161192</v>
+        <v>0.4548995333973023</v>
       </c>
       <c r="E19" t="n">
-        <v>0.118447103451176</v>
+        <v>0.1201240522613247</v>
       </c>
       <c r="F19" t="n">
-        <v>0.0310597546890643</v>
+        <v>0.02360726490118639</v>
       </c>
       <c r="G19" t="n">
-        <v>0.2329518292169372</v>
+        <v>0.1676019047645725</v>
       </c>
       <c r="H19" t="n">
         <v>0.1581413844293484</v>
@@ -2517,7 +1851,7 @@
         <v>0.2917299829957891</v>
       </c>
       <c r="J19" t="n">
-        <v>0.1503284191688047</v>
+        <v>0.1503572848465095</v>
       </c>
     </row>
     <row r="20">
@@ -2525,22 +1859,22 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>0.2030645865299134</v>
+        <v>0.3088879442164656</v>
       </c>
       <c r="C20" t="n">
-        <v>0.1940039501886527</v>
+        <v>0.2526787603062329</v>
       </c>
       <c r="D20" t="n">
-        <v>0.2576673421241071</v>
+        <v>0.1282058225918037</v>
       </c>
       <c r="E20" t="n">
-        <v>0.139101597646099</v>
+        <v>0.1830328459989394</v>
       </c>
       <c r="F20" t="n">
-        <v>0.2927497774051359</v>
+        <v>0.2654249183778162</v>
       </c>
       <c r="G20" t="n">
-        <v>0.2577745651171027</v>
+        <v>0.2478532841636987</v>
       </c>
       <c r="H20" t="n">
         <v>0.2667318017375011</v>
@@ -2549,7 +1883,7 @@
         <v>0.1458649914978946</v>
       </c>
       <c r="J20" t="n">
-        <v>0.1860585878440694</v>
+        <v>0.1860615958498842</v>
       </c>
     </row>
     <row r="21">
@@ -2557,22 +1891,22 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>0.3092245880609053</v>
+        <v>0.2384058630659404</v>
       </c>
       <c r="C21" t="n">
-        <v>0.3220073197481965</v>
+        <v>0.251974382144889</v>
       </c>
       <c r="D21" t="n">
-        <v>0.3039201827021045</v>
+        <v>0.1798785327149893</v>
       </c>
       <c r="E21" t="n">
-        <v>0.1272126077496682</v>
+        <v>0.173081542406469</v>
       </c>
       <c r="F21" t="n">
-        <v>0.1634113959387338</v>
+        <v>0.2271779123780381</v>
       </c>
       <c r="G21" t="n">
-        <v>0.2272235055476683</v>
+        <v>0.2351596820014379</v>
       </c>
       <c r="H21" t="n">
         <v>0.2098009033429356</v>
@@ -2581,7 +1915,7 @@
         <v>0.2917299829957891</v>
       </c>
       <c r="J21" t="n">
-        <v>0.1564867536414915</v>
+        <v>0.1564928082694497</v>
       </c>
     </row>
     <row r="22">
@@ -2589,22 +1923,22 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>0.05466639158109434</v>
+        <v>0.3524104057526262</v>
       </c>
       <c r="C22" t="n">
-        <v>9.750711460180557e-05</v>
+        <v>0.002817512645375388</v>
       </c>
       <c r="D22" t="n">
-        <v>1.942147449034374e-06</v>
+        <v>2.787988821642237e-06</v>
       </c>
       <c r="E22" t="n">
-        <v>0.2055666340383735</v>
+        <v>0.2077191264324403</v>
       </c>
       <c r="F22" t="n">
-        <v>0.5544398001212074</v>
+        <v>0.360320587117451</v>
       </c>
       <c r="G22" t="n">
-        <v>0.2825973010172681</v>
+        <v>0.2793453161265977</v>
       </c>
       <c r="H22" t="n">
         <v>0.3753222190456537</v>
@@ -2613,7 +1947,7 @@
         <v>0</v>
       </c>
       <c r="J22" t="n">
-        <v>0.2217887565193342</v>
+        <v>0.2217659068532589</v>
       </c>
     </row>
     <row r="23">
@@ -2621,22 +1955,22 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>0.3200663954085741</v>
+        <v>0.3057702867504717</v>
       </c>
       <c r="C23" t="n">
-        <v>0.3201181194027866</v>
+        <v>0.1973850746407409</v>
       </c>
       <c r="D23" t="n">
-        <v>0.2850145508089336</v>
+        <v>0.1305276847430411</v>
       </c>
       <c r="E23" t="n">
-        <v>0.1321457677351993</v>
+        <v>0.1840517451307557</v>
       </c>
       <c r="F23" t="n">
-        <v>0.2957630371884033</v>
+        <v>0.2699379638586017</v>
       </c>
       <c r="G23" t="n">
-        <v>0.2214951818783993</v>
+        <v>0.2468725556078921</v>
       </c>
       <c r="H23" t="n">
         <v>0.2614604222565228</v>
@@ -2645,7 +1979,7 @@
         <v>0.2917299829957891</v>
       </c>
       <c r="J23" t="n">
-        <v>0.1626450881141784</v>
+        <v>0.1626283316923899</v>
       </c>
     </row>
     <row r="24">
@@ -2653,22 +1987,22 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>0.3097289447958499</v>
+        <v>0.1295648545671958</v>
       </c>
       <c r="C24" t="n">
-        <v>0.3386522166742794</v>
+        <v>0.1959763183180532</v>
       </c>
       <c r="D24" t="n">
-        <v>0.3382391624722785</v>
+        <v>0.4855486150051087</v>
       </c>
       <c r="E24" t="n">
-        <v>0.1184348055594374</v>
+        <v>0.1196749388104001</v>
       </c>
       <c r="F24" t="n">
-        <v>0.03708627425559916</v>
+        <v>0.02410171151287297</v>
       </c>
       <c r="G24" t="n">
-        <v>0.1603930627395305</v>
+        <v>0.1585473415853663</v>
       </c>
       <c r="H24" t="n">
         <v>0.1475986254673919</v>
@@ -2677,7 +2011,7 @@
         <v>0.5834599659915782</v>
       </c>
       <c r="J24" t="n">
-        <v>0.1035014197090226</v>
+        <v>0.1034907565315208</v>
       </c>
     </row>
   </sheetData>
@@ -2809,27 +2143,27 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B2" t="n">
-        <v>0.6559971525283252</v>
+        <v>0.7463363240737964</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>$A_{06}$</t>
+          <t>$A_{20}$</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" t="n">
-        <v>0.6556862914393586</v>
+        <v>0.7041518351409056</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>$A_{13}$</t>
+          <t>$A_{12}$</t>
         </is>
       </c>
     </row>
@@ -2838,7 +2172,7 @@
         <v>21</v>
       </c>
       <c r="B4" t="n">
-        <v>0.644502543577697</v>
+        <v>0.6686491638330152</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -2848,248 +2182,248 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B5" t="n">
-        <v>0.6268906474075107</v>
+        <v>0.6679935278594124</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>$A_{11}$</t>
+          <t>$A_{18}$</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>0.623060647458326</v>
+        <v>0.6316117469828726</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>$A_{19}$</t>
+          <t>$A_{05}$</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B7" t="n">
-        <v>0.5949561580571848</v>
+        <v>0.6010987241691176</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>$A_{05}$</t>
+          <t>$A_{10}$</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B8" t="n">
-        <v>0.5929492944874826</v>
+        <v>0.6009135820115546</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>$A_{17}$</t>
+          <t>$A_{13}$</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="B9" t="n">
-        <v>0.5883710094648167</v>
+        <v>0.5924222469243355</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>$A_{22}$</t>
+          <t>$A_{04}$</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>0.5836831394744536</v>
+        <v>0.5674575694061066</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>$A_{12}$</t>
+          <t>$A_{09}$</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="B11" t="n">
-        <v>0.5531312462809661</v>
+        <v>0.5592817903305939</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>$A_{03}$</t>
+          <t>$A_{19}$</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B12" t="n">
-        <v>0.5516640671157687</v>
+        <v>0.5561588875607631</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>$A_{10}$</t>
+          <t>$A_{16}$</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>0.5376334604881771</v>
+        <v>0.527984412187778</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>$A_{18}$</t>
+          <t>$A_{15}$</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B14" t="n">
-        <v>0.5093042082692649</v>
+        <v>0.4816061659327805</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>$A_{08}$</t>
+          <t>$A_{02}$</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B15" t="n">
-        <v>0.5056804072833425</v>
+        <v>0.4498057847361142</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>$A_{16}$</t>
+          <t>$A_{07}$</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B16" t="n">
-        <v>0.4327488994624472</v>
+        <v>0.4404796202730473</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>$A_{00}$</t>
+          <t>$A_{03}$</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B17" t="n">
-        <v>0.413562859756012</v>
+        <v>0.4341778899976921</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>$A_{04}$</t>
+          <t>$A_{06}$</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="B18" t="n">
-        <v>0.4091353226482249</v>
+        <v>0.4131021327524648</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>$A_{20}$</t>
+          <t>$A_{00}$</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B19" t="n">
-        <v>0.3924295899897636</v>
+        <v>0.3987233666020975</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>$A_{02}$</t>
+          <t>$A_{11}$</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B20" t="n">
-        <v>0.3824125641752777</v>
+        <v>0.3983853655587689</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>$A_{09}$</t>
+          <t>$A_{08}$</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="B21" t="n">
-        <v>0.3694510101848137</v>
+        <v>0.3657469798772428</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>$A_{01}$</t>
+          <t>$A_{22}$</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B22" t="n">
-        <v>0.36151000377089</v>
+        <v>0.3553114066833757</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>$A_{07}$</t>
+          <t>$A_{01}$</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B23" t="n">
-        <v>0.3581786233471275</v>
+        <v>0.3490622424199212</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>$A_{15}$</t>
+          <t>$A_{17}$</t>
         </is>
       </c>
     </row>
@@ -3098,7 +2432,7 @@
         <v>14</v>
       </c>
       <c r="B24" t="n">
-        <v>0.3324390473858094</v>
+        <v>0.3138832727217861</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>

</xml_diff>